<commit_message>
closes #27: updated templates, cleaned file uploads, specified upload for each lab to avoid write conflict
</commit_message>
<xml_diff>
--- a/WF1_DevTemplate.xlsx
+++ b/WF1_DevTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36E071D-B558-6547-B89A-5BF6B62BFFBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B6A831-BD3C-4E44-A758-0D72F67B4C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26020" yWindow="460" windowWidth="25020" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11460" yWindow="460" windowWidth="39560" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WF1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="151">
   <si>
     <t>ExpWorkflowVer</t>
   </si>
@@ -223,12 +223,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> Lower [M] molar concentration for chem2 in any given portion for all experiments</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Upper [M] molar concentration for chem2 in any given portion for all experiments</t>
-  </si>
-  <si>
     <t>Reagent2_item1_formulaconc</t>
   </si>
   <si>
@@ -809,6 +803,62 @@
   </si>
   <si>
     <t>Reagent3_prep_duration</t>
+  </si>
+  <si>
+    <t>Not working in the current version - see git issue</t>
+  </si>
+  <si>
+    <t>Reagent2_ID</t>
+  </si>
+  <si>
+    <t>Model[Sample, StockSolution, "id:kEJ9mqR8n6WP"]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ECL model ID.  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cannot be used in with `Reagent#_chemical_list`</t>
+    </r>
+  </si>
+  <si>
+    <t>See 'Reagents' workbook</t>
+  </si>
+  <si>
+    <t>Reagent5_ID</t>
+  </si>
+  <si>
+    <t>Reagent6_ID</t>
+  </si>
+  <si>
+    <t>Reagent7_ID</t>
+  </si>
+  <si>
+    <t>Reagent4_ID</t>
+  </si>
+  <si>
+    <t>Reagent3_ID</t>
+  </si>
+  <si>
+    <t>Reagent1_ID</t>
+  </si>
+  <si>
+    <t>Model[Sample, Chemical, "Formic acid, reagent grade &gt;95%"]</t>
+  </si>
+  <si>
+    <t>Model[Sample, StockSolution, "id:xRO9n3BEG1Nw"]</t>
+  </si>
+  <si>
+    <t>Model[Sample, Chemical, "id:N80DNjlYwwAo"]</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1052,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1178,21 +1228,6 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1220,6 +1255,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1510,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1584,8 @@
     <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.83203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="41.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="91.5" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="92.1640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -1550,7 +1613,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1583,7 +1646,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H3" s="17"/>
     </row>
@@ -1605,7 +1668,7 @@
         <v>0</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H4" s="17"/>
     </row>
@@ -1627,7 +1690,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H5" s="27"/>
     </row>
@@ -1641,7 +1704,7 @@
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
       <c r="G6" s="31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H6" s="32"/>
     </row>
@@ -1663,7 +1726,7 @@
         <v>96</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H7" s="32"/>
     </row>
@@ -1685,10 +1748,10 @@
         <v>13</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1707,10 +1770,10 @@
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1729,10 +1792,10 @@
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1753,7 +1816,7 @@
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H11" s="32"/>
     </row>
@@ -1775,7 +1838,7 @@
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H12" s="32"/>
     </row>
@@ -1797,7 +1860,7 @@
       </c>
       <c r="F13" s="29"/>
       <c r="G13" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H13" s="32"/>
     </row>
@@ -1819,7 +1882,7 @@
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H14" s="32"/>
     </row>
@@ -1841,7 +1904,7 @@
       </c>
       <c r="F15" s="29"/>
       <c r="G15" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H15" s="32"/>
     </row>
@@ -1863,7 +1926,7 @@
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="31" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H16" s="32"/>
     </row>
@@ -1872,7 +1935,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>1</v>
@@ -1885,7 +1948,7 @@
       </c>
       <c r="F17" s="29"/>
       <c r="G17" s="31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H17" s="32"/>
     </row>
@@ -1894,7 +1957,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>1</v>
@@ -1907,35 +1970,35 @@
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="31" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H18" s="32"/>
     </row>
-    <row r="19" spans="1:8" s="66" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" s="61" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="C19" s="68" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="67">
+      <c r="B19" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="62">
         <v>24</v>
       </c>
-      <c r="E19" s="67" t="s">
+      <c r="E19" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="67"/>
-      <c r="G19" s="69" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="70"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="65"/>
     </row>
     <row r="20" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
@@ -1943,10 +2006,10 @@
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
       <c r="G20" s="37" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -1979,10 +2042,10 @@
         <v>0.1</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2005,10 +2068,10 @@
         <v>3</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="H23" s="38" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2031,10 +2094,10 @@
       <c r="E25" s="35"/>
       <c r="F25" s="35"/>
       <c r="G25" s="37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2046,403 +2109,409 @@
       <c r="F26" s="35"/>
       <c r="G26" s="37"/>
       <c r="H26" s="58" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="75" t="s">
-        <v>123</v>
+      <c r="D27" s="70" t="s">
+        <v>121</v>
       </c>
       <c r="E27" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="75" t="s">
-        <v>123</v>
+      <c r="F27" s="70" t="s">
+        <v>121</v>
       </c>
       <c r="G27" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="H27" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="H27" s="74" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="28" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="34"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="38"/>
+      <c r="A28" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="70" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="70" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="74" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="29" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
-      <c r="B29" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E29" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="H29" s="38" t="s">
-        <v>83</v>
-      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
     </row>
     <row r="30" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="34"/>
       <c r="B30" s="35" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="C30" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D30" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E30" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="H30" s="38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="70" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="E31" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="34"/>
+      <c r="B32" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="35">
         <v>2.2799999999999998</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E32" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="35">
+      <c r="F32" s="35">
         <v>3</v>
       </c>
-      <c r="G30" s="37" t="s">
-        <v>85</v>
-      </c>
-      <c r="H30" s="38" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="C31" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="35">
+      <c r="G32" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="H32" s="38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="34"/>
+      <c r="B33" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="35">
         <v>2.85</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E33" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="35">
+      <c r="F33" s="35">
         <v>1.5</v>
       </c>
-      <c r="G31" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="H31" s="38"/>
-    </row>
-    <row r="32" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="35">
-        <v>75</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="35">
-        <v>75</v>
-      </c>
-      <c r="G32" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H32" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="35">
-        <v>450</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="35">
-        <v>450</v>
-      </c>
       <c r="G33" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="H33" s="38" t="s">
-        <v>82</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="H33" s="38"/>
     </row>
     <row r="34" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="35">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="E34" s="35" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="35">
+        <v>75</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="35">
+        <v>450</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F35" s="35">
+        <v>450</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="35">
         <v>3600</v>
       </c>
-      <c r="G34" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="H34" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="34"/>
-      <c r="B35" s="35"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="38"/>
-    </row>
-    <row r="36" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="34"/>
-      <c r="B36" s="35" t="s">
-        <v>118</v>
-      </c>
-      <c r="C36" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" s="35" t="s">
-        <v>127</v>
-      </c>
       <c r="E36" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" s="35" t="s">
-        <v>127</v>
+        <v>21</v>
+      </c>
+      <c r="F36" s="35">
+        <v>3600</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="H36" s="38"/>
+        <v>79</v>
+      </c>
+      <c r="H36" s="38" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="37" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="34"/>
-      <c r="B37" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" s="35">
+      <c r="B37" s="35"/>
+      <c r="C37" s="36"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="38"/>
+    </row>
+    <row r="38" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="34"/>
+      <c r="B38" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="H38" s="38"/>
+    </row>
+    <row r="39" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="70" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="H39" s="74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="34"/>
+      <c r="B40" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="35">
         <v>4.18</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E40" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="F37" s="35">
+      <c r="F40" s="35">
         <v>6</v>
       </c>
-      <c r="G37" s="37" t="s">
-        <v>87</v>
-      </c>
-      <c r="H37" s="38"/>
-    </row>
-    <row r="38" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="C38" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="35">
+      <c r="G40" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" s="38"/>
+    </row>
+    <row r="41" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="35">
         <v>75</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E41" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F38" s="35">
+      <c r="F41" s="35">
         <v>75</v>
       </c>
-      <c r="G38" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H38" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="35">
-        <v>450</v>
-      </c>
-      <c r="E39" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="35">
-        <v>450</v>
-      </c>
-      <c r="G39" s="37" t="s">
+      <c r="G41" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="H39" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="35">
-        <v>3600</v>
-      </c>
-      <c r="E40" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F40" s="35">
-        <v>3600</v>
-      </c>
-      <c r="G40" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="H40" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="38"/>
     </row>
     <row r="42" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="C42" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="35" t="s">
-        <v>126</v>
+      <c r="D42" s="35">
+        <v>450</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="35" t="s">
-        <v>126</v>
+        <v>21</v>
+      </c>
+      <c r="F42" s="35">
+        <v>450</v>
       </c>
       <c r="G42" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42" s="38"/>
+        <v>78</v>
+      </c>
+      <c r="H42" s="38" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="43" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="44" t="s">
-        <v>61</v>
+      <c r="B43" s="35" t="s">
+        <v>136</v>
       </c>
       <c r="C43" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="35">
-        <v>2</v>
+        <v>3600</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F43" s="35">
-        <v>2</v>
+        <v>3600</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>94</v>
-      </c>
-      <c r="H43" s="38"/>
+        <v>79</v>
+      </c>
+      <c r="H43" s="38" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="44" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D44" s="35">
-        <v>1.4</v>
-      </c>
-      <c r="E44" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F44" s="35">
-        <v>1</v>
-      </c>
-      <c r="G44" s="37" t="s">
-        <v>93</v>
-      </c>
+      <c r="A44" s="34"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="36"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="37"/>
       <c r="H44" s="38"/>
     </row>
     <row r="45" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2450,89 +2519,97 @@
         <v>14</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="C45" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="35">
-        <v>75</v>
+      <c r="D45" s="35" t="s">
+        <v>124</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="35">
-        <v>75</v>
+        <v>49</v>
+      </c>
+      <c r="F45" s="35" t="s">
+        <v>124</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H45" s="38" t="s">
-        <v>82</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H45" s="38"/>
     </row>
     <row r="46" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="C46" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="35">
-        <v>450</v>
-      </c>
-      <c r="E46" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46" s="35">
-        <v>450</v>
-      </c>
-      <c r="G46" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="H46" s="38" t="s">
-        <v>82</v>
+      <c r="A46" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="70" t="s">
+        <v>139</v>
+      </c>
+      <c r="G46" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="H46" s="74" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="35" t="s">
-        <v>135</v>
+      <c r="B47" s="44" t="s">
+        <v>59</v>
       </c>
       <c r="C47" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D47" s="35">
-        <v>3600</v>
+        <v>2</v>
       </c>
       <c r="E47" s="35" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F47" s="35">
-        <v>3600</v>
+        <v>2</v>
       </c>
       <c r="G47" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="H47" s="38" t="s">
-        <v>82</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="H47" s="38"/>
     </row>
     <row r="48" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="37"/>
+      <c r="B48" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="35">
+        <v>1.4</v>
+      </c>
+      <c r="E48" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" s="35">
+        <v>1</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>91</v>
+      </c>
       <c r="H48" s="38"/>
     </row>
     <row r="49" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -2540,499 +2617,674 @@
         <v>14</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C49" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="35" t="s">
-        <v>127</v>
+      <c r="D49" s="35">
+        <v>75</v>
       </c>
       <c r="E49" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="35" t="s">
-        <v>127</v>
+        <v>21</v>
+      </c>
+      <c r="F49" s="35">
+        <v>75</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="H49" s="38"/>
+        <v>77</v>
+      </c>
+      <c r="H49" s="38" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="50" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="44" t="s">
-        <v>63</v>
+      <c r="B50" s="35" t="s">
+        <v>132</v>
       </c>
       <c r="C50" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="35">
-        <v>7.4</v>
+        <v>450</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F50" s="35">
-        <v>4.5</v>
+        <v>450</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>95</v>
-      </c>
-      <c r="H50" s="38"/>
+        <v>78</v>
+      </c>
+      <c r="H50" s="38" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="51" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C51" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="35">
-        <v>75</v>
+        <v>3600</v>
       </c>
       <c r="E51" s="35" t="s">
         <v>21</v>
       </c>
       <c r="F51" s="35">
-        <v>75</v>
+        <v>3600</v>
       </c>
       <c r="G51" s="37" t="s">
         <v>79</v>
       </c>
       <c r="H51" s="38" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B52" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="C52" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D52" s="35">
-        <v>450</v>
-      </c>
-      <c r="E52" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F52" s="35">
-        <v>450</v>
-      </c>
-      <c r="G52" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="H52" s="38" t="s">
-        <v>82</v>
-      </c>
+      <c r="B52" s="35"/>
+      <c r="C52" s="36"/>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
     </row>
     <row r="53" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B53" s="35" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="C53" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="35">
+      <c r="D53" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="F53" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="G53" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="H53" s="38"/>
+    </row>
+    <row r="54" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="70" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="E54" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="70" t="s">
+        <v>149</v>
+      </c>
+      <c r="G54" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="H54" s="74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="35">
+        <v>7.4</v>
+      </c>
+      <c r="E55" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="F55" s="35">
+        <v>4.5</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="H55" s="38"/>
+    </row>
+    <row r="56" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D56" s="35">
+        <v>75</v>
+      </c>
+      <c r="E56" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F56" s="35">
+        <v>75</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="H56" s="38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="35">
+        <v>450</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="F57" s="35">
+        <v>450</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H57" s="38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="35">
         <v>3600</v>
       </c>
-      <c r="E53" s="35" t="s">
+      <c r="E58" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F53" s="35">
+      <c r="F58" s="35">
         <v>3600</v>
       </c>
-      <c r="G53" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="H53" s="38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="34"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="38"/>
-    </row>
-    <row r="55" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="34"/>
-      <c r="B55" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="E55" s="35" t="s">
+      <c r="G58" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H58" s="38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="34"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="38"/>
+    </row>
+    <row r="60" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="34"/>
+      <c r="B60" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E60" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F55" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="G55" s="37" t="s">
+      <c r="F60" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G60" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H55" s="38"/>
-    </row>
-    <row r="56" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="37"/>
-      <c r="H56" s="38"/>
-    </row>
-    <row r="57" spans="1:8" s="66" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="62"/>
-      <c r="B57" s="63" t="s">
-        <v>117</v>
-      </c>
-      <c r="C57" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="63" t="s">
-        <v>128</v>
-      </c>
-      <c r="E57" s="63" t="s">
+      <c r="H60" s="38"/>
+    </row>
+    <row r="61" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="70" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="70" t="s">
+        <v>148</v>
+      </c>
+      <c r="G61" s="73" t="s">
+        <v>140</v>
+      </c>
+      <c r="H61" s="74" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="34"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="36"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="38"/>
+    </row>
+    <row r="63" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="34"/>
+      <c r="B63" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="E63" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F57" s="63" t="s">
-        <v>128</v>
-      </c>
-      <c r="G57" s="61" t="s">
+      <c r="F63" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G63" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="65"/>
-    </row>
-    <row r="58" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="46" t="s">
+      <c r="H63" s="38"/>
+    </row>
+    <row r="64" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" s="76" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="E64" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="76" t="s">
+        <v>148</v>
+      </c>
+      <c r="G64" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="H64" s="79" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B58" s="47"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="50"/>
-    </row>
-    <row r="59" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="46"/>
-      <c r="B59" s="47" t="s">
+      <c r="B65" s="47"/>
+      <c r="C65" s="48"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="50"/>
+    </row>
+    <row r="66" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="46"/>
+      <c r="B66" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="C59" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D59" s="47">
+      <c r="C66" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="47">
         <v>750</v>
       </c>
-      <c r="E59" s="47" t="s">
+      <c r="E66" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F59" s="47">
+      <c r="F66" s="47">
         <v>750</v>
       </c>
-      <c r="G59" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="H59" s="50"/>
-    </row>
-    <row r="60" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="46"/>
-      <c r="B60" s="47" t="s">
+      <c r="G66" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="H66" s="50"/>
+    </row>
+    <row r="67" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="46"/>
+      <c r="B67" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="47">
+      <c r="C67" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="47">
         <v>80</v>
       </c>
-      <c r="E60" s="47" t="s">
+      <c r="E67" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="F60" s="47">
+      <c r="F67" s="47">
         <v>80</v>
       </c>
-      <c r="G60" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="H60" s="50"/>
-    </row>
-    <row r="61" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="46"/>
-      <c r="B61" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C61" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="47">
-        <v>900</v>
-      </c>
-      <c r="E61" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F61" s="47">
-        <v>900</v>
-      </c>
-      <c r="G61" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="H61" s="50"/>
-    </row>
-    <row r="62" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="46"/>
-      <c r="B62" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D62" s="47">
-        <v>1200</v>
-      </c>
-      <c r="E62" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" s="47">
-        <v>1200</v>
-      </c>
-      <c r="G62" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H62" s="50"/>
-    </row>
-    <row r="63" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="46"/>
-      <c r="B63" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="C63" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D63" s="47">
-        <v>105</v>
-      </c>
-      <c r="E63" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="47">
-        <v>105</v>
-      </c>
-      <c r="G63" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="H63" s="50" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="46"/>
-      <c r="B64" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="C64" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="47">
-        <v>12600</v>
-      </c>
-      <c r="E64" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F64" s="47">
-        <v>12600</v>
-      </c>
-      <c r="G64" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="H64" s="50" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="46"/>
-      <c r="B65" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D65" s="47">
-        <v>3</v>
-      </c>
-      <c r="E65" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="F65" s="47">
-        <v>3</v>
-      </c>
-      <c r="G65" s="71" t="s">
-        <v>102</v>
-      </c>
-      <c r="H65" s="50" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="52"/>
-      <c r="B66" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D66" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="E66" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" s="53"/>
-      <c r="G66" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="H66" s="57" t="s">
+      <c r="G67" s="49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B67" s="47"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="49"/>
       <c r="H67" s="50"/>
     </row>
     <row r="68" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="46"/>
       <c r="B68" s="47" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C68" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D68" s="47">
-        <v>45</v>
+        <v>900</v>
       </c>
       <c r="E68" s="47" t="s">
         <v>21</v>
       </c>
       <c r="F68" s="47">
-        <v>45</v>
+        <v>900</v>
       </c>
       <c r="G68" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H68" s="72" t="s">
-        <v>104</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="H68" s="50"/>
     </row>
     <row r="69" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="46"/>
       <c r="B69" s="47" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C69" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D69" s="47">
-        <v>75</v>
+        <v>1200</v>
       </c>
       <c r="E69" s="47" t="s">
         <v>21</v>
       </c>
       <c r="F69" s="47">
-        <v>75</v>
+        <v>1200</v>
       </c>
       <c r="G69" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="H69" s="72" t="s">
-        <v>104</v>
-      </c>
+      <c r="H69" s="50"/>
     </row>
     <row r="70" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="46"/>
       <c r="B70" s="47" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C70" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="47">
-        <v>450</v>
+        <v>105</v>
       </c>
       <c r="E70" s="47" t="s">
         <v>21</v>
       </c>
       <c r="F70" s="47">
+        <v>105</v>
+      </c>
+      <c r="G70" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="H70" s="50" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="46"/>
+      <c r="B71" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C71" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="47">
+        <v>12600</v>
+      </c>
+      <c r="E71" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F71" s="47">
+        <v>12600</v>
+      </c>
+      <c r="G71" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="H71" s="50" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="46"/>
+      <c r="B72" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C72" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="47">
+        <v>3</v>
+      </c>
+      <c r="E72" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F72" s="47">
+        <v>3</v>
+      </c>
+      <c r="G72" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="H72" s="50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="52"/>
+      <c r="B73" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73" s="53" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="53"/>
+      <c r="G73" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="H73" s="57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B74" s="47"/>
+      <c r="C74" s="48"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="49"/>
+      <c r="H74" s="50"/>
+    </row>
+    <row r="75" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="46"/>
+      <c r="B75" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75" s="47">
+        <v>45</v>
+      </c>
+      <c r="E75" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F75" s="47">
+        <v>45</v>
+      </c>
+      <c r="G75" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="H75" s="67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="46"/>
+      <c r="B76" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C76" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" s="47">
+        <v>75</v>
+      </c>
+      <c r="E76" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F76" s="47">
+        <v>75</v>
+      </c>
+      <c r="G76" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H76" s="67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="46"/>
+      <c r="B77" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C77" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77" s="47">
         <v>450</v>
       </c>
-      <c r="G70" s="49" t="s">
+      <c r="E77" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="F77" s="47">
+        <v>450</v>
+      </c>
+      <c r="G77" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H77" s="67" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="52"/>
+      <c r="B78" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D78" s="53">
+        <v>3600</v>
+      </c>
+      <c r="E78" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78" s="53">
+        <v>3600</v>
+      </c>
+      <c r="G78" s="56" t="s">
         <v>105</v>
       </c>
-      <c r="H70" s="72" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="52"/>
-      <c r="B71" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="C71" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" s="53">
-        <v>3600</v>
-      </c>
-      <c r="E71" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71" s="53">
-        <v>3600</v>
-      </c>
-      <c r="G71" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="H71" s="73" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H78" s="68" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H26" r:id="rId1" xr:uid="{BFFDF1DF-AC10-154F-90C8-6E1B425878BE}"/>
+    <hyperlink ref="H31" r:id="rId2" xr:uid="{0E829C9D-F5CA-C344-BA01-6E533C5654BA}"/>
+    <hyperlink ref="H39" r:id="rId3" xr:uid="{A121E58C-073A-E143-9B04-5E9274078D9A}"/>
+    <hyperlink ref="H28" r:id="rId4" xr:uid="{B982A0B7-E477-1C4F-8364-A396A3924E00}"/>
+    <hyperlink ref="H46" r:id="rId5" xr:uid="{405EB354-6600-474D-853F-66209B7460CD}"/>
+    <hyperlink ref="H54" r:id="rId6" xr:uid="{4E8679E9-B210-6348-ADD3-3F77E2C8E25A}"/>
+    <hyperlink ref="H61" r:id="rId7" xr:uid="{8568EC0E-EC0D-F24E-843E-31850DCF03B6}"/>
+    <hyperlink ref="H64" r:id="rId8" xr:uid="{91A8231D-5654-B04D-A342-76461EC7B009}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Toward #32, closes #48 mathematica sampling no WF3 support
</commit_message>
<xml_diff>
--- a/WF1_DevTemplate.xlsx
+++ b/WF1_DevTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B6A831-BD3C-4E44-A758-0D72F67B4C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520479B-09EC-FA4C-BADF-5C05DCD015DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="460" windowWidth="39560" windowHeight="27640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11460" yWindow="460" windowWidth="39560" windowHeight="27560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WF1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" calcOnSave="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="147">
   <si>
     <t>ExpWorkflowVer</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Actions (Experiments)</t>
   </si>
   <si>
-    <t>[[4,5,1],[6,7]]</t>
-  </si>
-  <si>
-    <t>[[3000,3000],[1000,1000]]</t>
-  </si>
-  <si>
     <t>exp2</t>
   </si>
   <si>
@@ -73,12 +67,6 @@
     <t>exp2_wells</t>
   </si>
   <si>
-    <t>exp3</t>
-  </si>
-  <si>
-    <t>exp3_vols</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -115,9 +103,6 @@
     <t>plotter_on</t>
   </si>
   <si>
-    <t>[[500,500],[0,250]]</t>
-  </si>
-  <si>
     <t>wellcount</t>
   </si>
   <si>
@@ -128,9 +113,6 @@
   </si>
   <si>
     <t>exp1_wells</t>
-  </si>
-  <si>
-    <t>exp3_wells</t>
   </si>
   <si>
     <t>stirrate</t>
@@ -745,15 +727,6 @@
     </r>
   </si>
   <si>
-    <t>exp4</t>
-  </si>
-  <si>
-    <t>exp4_vols</t>
-  </si>
-  <si>
-    <t>exp4_wells</t>
-  </si>
-  <si>
     <t>Primary solvent for experiments - GBL, DMSO, etc</t>
   </si>
   <si>
@@ -859,6 +832,21 @@
   </si>
   <si>
     <t>Model[Sample, Chemical, "id:N80DNjlYwwAo"]</t>
+  </si>
+  <si>
+    <t>[[2,3,1,7]]</t>
+  </si>
+  <si>
+    <t>[[500,500]]</t>
+  </si>
+  <si>
+    <t>[[4,5,1,7]]</t>
+  </si>
+  <si>
+    <t>['PbI2','AcNH3I','GBL']</t>
+  </si>
+  <si>
+    <t>['AcNH3I','GBL']</t>
   </si>
 </sst>
 </file>
@@ -953,7 +941,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1018,28 +1006,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -1228,28 +1194,13 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1281,6 +1232,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1572,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1592,7 +1558,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>5</v>
@@ -1601,24 +1567,24 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="15"/>
@@ -1640,20 +1606,20 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3" s="14">
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H3" s="17"/>
     </row>
     <row r="4" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>1</v>
@@ -1662,41 +1628,41 @@
         <v>0</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F4" s="20">
         <v>0</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H4" s="17"/>
     </row>
     <row r="5" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="30"/>
@@ -1704,14 +1670,14 @@
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
       <c r="G6" s="31" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28"/>
       <c r="B7" s="29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>1</v>
@@ -1720,1267 +1686,1255 @@
         <v>96</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" s="29">
         <v>96</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H7" s="32"/>
     </row>
     <row r="8" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="28"/>
       <c r="B8" s="29" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H8" s="32" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="28"/>
       <c r="B9" s="29" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F9" s="29"/>
       <c r="G9" s="31" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H9" s="32" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="28"/>
       <c r="B10" s="29" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="29">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="31" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H10" s="32" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="28"/>
       <c r="B11" s="29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F11" s="29"/>
       <c r="G11" s="31" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H11" s="32"/>
     </row>
     <row r="12" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="28" t="s">
-        <v>14</v>
-      </c>
+      <c r="A12" s="28"/>
       <c r="B12" s="29" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>11</v>
+        <v>143</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F12" s="29"/>
       <c r="G12" s="31" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H12" s="32"/>
     </row>
-    <row r="13" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="75"/>
+      <c r="B13" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="29">
-        <v>24</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="32"/>
+      <c r="C13" s="77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="76">
+        <v>48</v>
+      </c>
+      <c r="E13" s="76" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="76"/>
+      <c r="G13" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="31" t="s">
+      <c r="A14" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="H14" s="38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+    </row>
+    <row r="16" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="35">
+        <v>0.2</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="40">
+        <v>3</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="60"/>
+    </row>
+    <row r="19" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="32"/>
-    </row>
-    <row r="15" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="H15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="29">
-        <v>24</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" s="32"/>
-    </row>
-    <row r="17" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" s="32"/>
-    </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" s="32"/>
-    </row>
-    <row r="19" spans="1:8" s="61" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19" s="63" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" s="62">
-        <v>24</v>
-      </c>
-      <c r="E19" s="62" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="62"/>
-      <c r="G19" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="65"/>
     </row>
     <row r="20" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="34" t="s">
-        <v>111</v>
-      </c>
+      <c r="A20" s="34"/>
       <c r="B20" s="35"/>
       <c r="C20" s="36"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="38" t="s">
-        <v>88</v>
+      <c r="G20" s="37"/>
+      <c r="H20" s="58" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="34"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
+      <c r="B21" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>111</v>
+      </c>
+      <c r="H21" s="64" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="35">
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="H22" s="38" t="s">
-        <v>107</v>
+      <c r="A22" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="65" t="s">
+        <v>138</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="G22" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="H22" s="69" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B23" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="35">
-        <v>1.5</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="40">
-        <v>3</v>
-      </c>
-      <c r="G23" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="H23" s="38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="41"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="60"/>
+      <c r="A23" s="34"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
+    </row>
+    <row r="24" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="34"/>
+      <c r="B24" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="25" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="38" t="s">
-        <v>75</v>
+      <c r="A25" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C25" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E25" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="69" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="34"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="58" t="s">
-        <v>123</v>
+      <c r="B26" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="35">
+        <v>3</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="35" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="70" t="s">
-        <v>121</v>
+      <c r="D27" s="35">
+        <v>3</v>
       </c>
       <c r="E27" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="G27" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="38"/>
+    </row>
+    <row r="28" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="70" t="s">
-        <v>121</v>
-      </c>
-      <c r="G27" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="H27" s="69" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B28" s="70" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="E28" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="70" t="s">
-        <v>150</v>
-      </c>
-      <c r="G28" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="H28" s="74" t="s">
-        <v>141</v>
+      <c r="C28" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="35">
+        <v>75</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="35">
+        <v>75</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="38" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="34"/>
-      <c r="B29" s="35"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="38"/>
+      <c r="A29" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="35">
+        <v>450</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="35">
+        <v>450</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="38" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="30" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="34"/>
+      <c r="A30" s="34" t="s">
+        <v>12</v>
+      </c>
       <c r="B30" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>124</v>
+        <v>51</v>
+      </c>
+      <c r="C30" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="35">
+        <v>3600</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>124</v>
+        <v>17</v>
+      </c>
+      <c r="F30" s="35">
+        <v>3600</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="H30" s="38" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="70" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="E31" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="G31" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="H31" s="74" t="s">
-        <v>141</v>
-      </c>
+      <c r="A31" s="34"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="36"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
     </row>
     <row r="32" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="34"/>
       <c r="B32" s="35" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="C32" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D32" s="35">
-        <v>2.2799999999999998</v>
+      <c r="D32" s="35" t="s">
+        <v>116</v>
       </c>
       <c r="E32" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="35">
-        <v>3</v>
+        <v>43</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>116</v>
       </c>
       <c r="G32" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="38" t="s">
-        <v>108</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="H32" s="38"/>
     </row>
     <row r="33" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
-      <c r="B33" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="35">
-        <v>2.85</v>
-      </c>
-      <c r="E33" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F33" s="35">
-        <v>1.5</v>
-      </c>
-      <c r="G33" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="H33" s="38"/>
+      <c r="A33" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="G33" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="H33" s="69" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="34" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="36" t="s">
+      <c r="A34" s="34"/>
+      <c r="B34" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="39" t="s">
         <v>1</v>
       </c>
       <c r="D34" s="35">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="E34" s="35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F34" s="35">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="G34" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="38" t="s">
-        <v>80</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H34" s="38"/>
     </row>
     <row r="35" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B35" s="35" t="s">
-        <v>56</v>
+        <v>125</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D35" s="35">
-        <v>450</v>
+        <v>75</v>
       </c>
       <c r="E35" s="35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F35" s="35">
-        <v>450</v>
+        <v>75</v>
       </c>
       <c r="G35" s="37" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H35" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>57</v>
+        <v>126</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D36" s="35">
+        <v>450</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="35">
+        <v>450</v>
+      </c>
+      <c r="G36" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H36" s="38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="35">
         <v>3600</v>
       </c>
-      <c r="E36" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="35">
+      <c r="E37" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="35">
         <v>3600</v>
       </c>
-      <c r="G36" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H36" s="38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34"/>
-      <c r="B37" s="35"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="35"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="38"/>
+      <c r="G37" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H37" s="38" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="38" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="34"/>
-      <c r="B38" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="E38" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="G38" s="37" t="s">
-        <v>82</v>
-      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="36"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="37"/>
       <c r="H38" s="38"/>
     </row>
     <row r="39" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B39" s="70" t="s">
-        <v>146</v>
-      </c>
-      <c r="C39" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D39" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="E39" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="G39" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="H39" s="74" t="s">
-        <v>141</v>
-      </c>
+      <c r="A39" s="34"/>
+      <c r="B39" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39" s="38"/>
     </row>
     <row r="40" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="34"/>
-      <c r="B40" s="44" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="35">
-        <v>4.18</v>
-      </c>
-      <c r="E40" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="35">
-        <v>6</v>
-      </c>
-      <c r="G40" s="37" t="s">
+      <c r="A40" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="E40" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="65" t="s">
+        <v>130</v>
+      </c>
+      <c r="G40" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="H40" s="69" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="34"/>
+      <c r="B41" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="35">
+        <v>2</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="H41" s="38"/>
+    </row>
+    <row r="42" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="34"/>
+      <c r="B42" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="35">
+        <v>0.38</v>
+      </c>
+      <c r="E42" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="35">
+        <v>1</v>
+      </c>
+      <c r="G42" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="H40" s="38"/>
-    </row>
-    <row r="41" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="35" t="s">
-        <v>134</v>
-      </c>
-      <c r="C41" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41" s="35">
-        <v>75</v>
-      </c>
-      <c r="E41" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" s="35">
-        <v>75</v>
-      </c>
-      <c r="G41" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="H41" s="38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>135</v>
-      </c>
-      <c r="C42" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="35">
-        <v>450</v>
-      </c>
-      <c r="E42" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="35">
-        <v>450</v>
-      </c>
-      <c r="G42" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="H42" s="38" t="s">
-        <v>80</v>
-      </c>
+      <c r="H42" s="38"/>
     </row>
     <row r="43" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B43" s="35" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C43" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D43" s="35">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F43" s="35">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="G43" s="37" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H43" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="34"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="38"/>
+      <c r="A44" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C44" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="35">
+        <v>450</v>
+      </c>
+      <c r="E44" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="35">
+        <v>450</v>
+      </c>
+      <c r="G44" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="H44" s="38" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="45" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B45" s="35" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="C45" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D45" s="35" t="s">
-        <v>124</v>
+      <c r="D45" s="35">
+        <v>3600</v>
       </c>
       <c r="E45" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" s="35" t="s">
-        <v>124</v>
+        <v>17</v>
+      </c>
+      <c r="F45" s="35">
+        <v>3600</v>
       </c>
       <c r="G45" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="H45" s="38"/>
+        <v>73</v>
+      </c>
+      <c r="H45" s="38" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="46" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="70" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D46" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="E46" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="70" t="s">
-        <v>139</v>
-      </c>
-      <c r="G46" s="73" t="s">
+      <c r="A46" s="34"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="36"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+    </row>
+    <row r="47" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="34"/>
+      <c r="B47" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F47" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" s="38"/>
+    </row>
+    <row r="48" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="65" t="s">
         <v>140</v>
       </c>
-      <c r="H46" s="74" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B47" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D47" s="35">
-        <v>2</v>
-      </c>
-      <c r="E47" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F47" s="35">
-        <v>2</v>
-      </c>
-      <c r="G47" s="37" t="s">
-        <v>92</v>
-      </c>
-      <c r="H47" s="38"/>
-    </row>
-    <row r="48" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B48" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D48" s="35">
-        <v>1.4</v>
-      </c>
-      <c r="E48" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F48" s="35">
-        <v>1</v>
-      </c>
-      <c r="G48" s="37" t="s">
-        <v>91</v>
-      </c>
-      <c r="H48" s="38"/>
+      <c r="E48" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="G48" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="H48" s="69" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="49" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="35" t="s">
-        <v>131</v>
+      <c r="A49" s="34"/>
+      <c r="B49" s="44" t="s">
+        <v>55</v>
       </c>
       <c r="C49" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D49" s="35">
-        <v>75</v>
+        <v>5.84</v>
       </c>
       <c r="E49" s="35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F49" s="35">
-        <v>75</v>
+        <v>4.5</v>
       </c>
       <c r="G49" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="H49" s="38" t="s">
-        <v>80</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="H49" s="38"/>
     </row>
     <row r="50" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B50" s="35" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C50" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D50" s="35">
-        <v>450</v>
+        <v>75</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F50" s="35">
-        <v>450</v>
+        <v>75</v>
       </c>
       <c r="G50" s="37" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="H50" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B51" s="35" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C51" s="36" t="s">
         <v>1</v>
       </c>
       <c r="D51" s="35">
-        <v>3600</v>
+        <v>450</v>
       </c>
       <c r="E51" s="35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F51" s="35">
-        <v>3600</v>
+        <v>450</v>
       </c>
       <c r="G51" s="37" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="H51" s="38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="38"/>
+        <v>12</v>
+      </c>
+      <c r="B52" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="35">
+        <v>3600</v>
+      </c>
+      <c r="E52" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="35">
+        <v>3600</v>
+      </c>
+      <c r="G52" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="H52" s="38" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="53" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B53" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="E53" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F53" s="35" t="s">
-        <v>125</v>
-      </c>
-      <c r="G53" s="37" t="s">
-        <v>3</v>
-      </c>
+      <c r="A53" s="34"/>
+      <c r="B53" s="35"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="35"/>
+      <c r="E53" s="35"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="37"/>
       <c r="H53" s="38"/>
     </row>
     <row r="54" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B54" s="70" t="s">
-        <v>142</v>
-      </c>
-      <c r="C54" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D54" s="70" t="s">
-        <v>149</v>
-      </c>
-      <c r="E54" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="70" t="s">
-        <v>149</v>
-      </c>
-      <c r="G54" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="H54" s="74" t="s">
-        <v>141</v>
-      </c>
+      <c r="A54" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D54" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F54" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="H54" s="38"/>
     </row>
     <row r="55" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B55" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="C55" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="35">
-        <v>7.4</v>
-      </c>
-      <c r="E55" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="F55" s="35">
-        <v>4.5</v>
-      </c>
-      <c r="G55" s="37" t="s">
-        <v>93</v>
-      </c>
-      <c r="H55" s="38"/>
+      <c r="A55" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="65" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D55" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="F55" s="65" t="s">
+        <v>139</v>
+      </c>
+      <c r="G55" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="H55" s="69" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="56" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B56" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="C56" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D56" s="35">
-        <v>75</v>
-      </c>
-      <c r="E56" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F56" s="35">
-        <v>75</v>
-      </c>
-      <c r="G56" s="37" t="s">
-        <v>77</v>
-      </c>
-      <c r="H56" s="38" t="s">
+      <c r="A56" s="34"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="36"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="38"/>
+    </row>
+    <row r="57" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="34"/>
+      <c r="B57" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="G57" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="H57" s="38"/>
+    </row>
+    <row r="58" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="G58" s="73" t="s">
+        <v>131</v>
+      </c>
+      <c r="H58" s="74" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="47"/>
+      <c r="C59" s="48"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="50"/>
+    </row>
+    <row r="60" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="46"/>
+      <c r="B60" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="47">
+        <v>750</v>
+      </c>
+      <c r="E60" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="47">
+        <v>750</v>
+      </c>
+      <c r="G60" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="H60" s="50"/>
+    </row>
+    <row r="61" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="46"/>
+      <c r="B61" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="47">
         <v>80</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D57" s="35">
-        <v>450</v>
-      </c>
-      <c r="E57" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F57" s="35">
-        <v>450</v>
-      </c>
-      <c r="G57" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="H57" s="38" t="s">
+      <c r="E61" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" s="47">
         <v>80</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="C58" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="35">
-        <v>3600</v>
-      </c>
-      <c r="E58" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="F58" s="35">
-        <v>3600</v>
-      </c>
-      <c r="G58" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H58" s="38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="34"/>
-      <c r="B59" s="35"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="38"/>
-    </row>
-    <row r="60" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="34"/>
-      <c r="B60" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="C60" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="G60" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H60" s="38"/>
-    </row>
-    <row r="61" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="71" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" s="70" t="s">
-        <v>143</v>
-      </c>
-      <c r="C61" s="72" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="E61" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="70" t="s">
-        <v>148</v>
-      </c>
-      <c r="G61" s="73" t="s">
-        <v>140</v>
-      </c>
-      <c r="H61" s="74" t="s">
-        <v>141</v>
-      </c>
+      <c r="G61" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="50"/>
     </row>
     <row r="62" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="35"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="38"/>
+      <c r="A62" s="46"/>
+      <c r="B62" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" s="47">
+        <v>900</v>
+      </c>
+      <c r="E62" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F62" s="47">
+        <v>900</v>
+      </c>
+      <c r="G62" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="H62" s="50"/>
     </row>
     <row r="63" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="34"/>
-      <c r="B63" s="35" t="s">
-        <v>115</v>
-      </c>
-      <c r="C63" s="36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D63" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="E63" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="F63" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="G63" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="H63" s="38"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D63" s="47">
+        <v>1200</v>
+      </c>
+      <c r="E63" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="47">
+        <v>1200</v>
+      </c>
+      <c r="G63" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="H63" s="50"/>
     </row>
     <row r="64" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="75" t="s">
-        <v>14</v>
-      </c>
-      <c r="B64" s="76" t="s">
-        <v>144</v>
-      </c>
-      <c r="C64" s="77" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="76" t="s">
-        <v>148</v>
-      </c>
-      <c r="E64" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" s="76" t="s">
-        <v>148</v>
-      </c>
-      <c r="G64" s="78" t="s">
-        <v>140</v>
-      </c>
-      <c r="H64" s="79" t="s">
-        <v>141</v>
+      <c r="A64" s="46"/>
+      <c r="B64" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D64" s="47">
+        <v>105</v>
+      </c>
+      <c r="E64" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" s="47">
+        <v>105</v>
+      </c>
+      <c r="G64" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="H64" s="50" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B65" s="47"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="50"/>
+      <c r="A65" s="46"/>
+      <c r="B65" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="47">
+        <v>12600</v>
+      </c>
+      <c r="E65" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" s="47">
+        <v>12600</v>
+      </c>
+      <c r="G65" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="H65" s="50" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="66" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="46"/>
@@ -2991,298 +2945,162 @@
         <v>1</v>
       </c>
       <c r="D66" s="47">
-        <v>750</v>
+        <v>3</v>
       </c>
       <c r="E66" s="47" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F66" s="47">
-        <v>750</v>
-      </c>
-      <c r="G66" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="H66" s="50"/>
-    </row>
-    <row r="67" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="46"/>
-      <c r="B67" s="47" t="s">
+        <v>3</v>
+      </c>
+      <c r="G66" s="61" t="s">
+        <v>94</v>
+      </c>
+      <c r="H66" s="50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="52"/>
+      <c r="B67" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="C67" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67" s="47">
+      <c r="C67" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67" s="55" t="s">
+        <v>44</v>
+      </c>
+      <c r="E67" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="53"/>
+      <c r="G67" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="E67" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F67" s="47">
-        <v>80</v>
-      </c>
-      <c r="G67" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="H67" s="50"/>
+      <c r="H67" s="57" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="68" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="46"/>
-      <c r="B68" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="C68" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="47">
-        <v>900</v>
-      </c>
-      <c r="E68" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F68" s="47">
-        <v>900</v>
-      </c>
-      <c r="G68" s="49" t="s">
-        <v>94</v>
-      </c>
+      <c r="A68" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="47"/>
+      <c r="C68" s="48"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="49"/>
       <c r="H68" s="50"/>
     </row>
     <row r="69" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="46"/>
       <c r="B69" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C69" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D69" s="47">
-        <v>1200</v>
+        <v>45</v>
       </c>
       <c r="E69" s="47" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F69" s="47">
-        <v>1200</v>
+        <v>45</v>
       </c>
       <c r="G69" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="H69" s="50"/>
+        <v>95</v>
+      </c>
+      <c r="H69" s="62" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="70" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="46"/>
       <c r="B70" s="47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C70" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D70" s="47">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="E70" s="47" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F70" s="47">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="G70" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="H70" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="H70" s="62" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="46"/>
       <c r="B71" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71" s="47">
+        <v>450</v>
+      </c>
+      <c r="E71" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="47">
+        <v>450</v>
+      </c>
+      <c r="G71" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="52"/>
+      <c r="B72" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="C71" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71" s="47">
-        <v>12600</v>
-      </c>
-      <c r="E71" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F71" s="47">
-        <v>12600</v>
-      </c>
-      <c r="G71" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="H71" s="50" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="46"/>
-      <c r="B72" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="C72" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="47">
-        <v>3</v>
-      </c>
-      <c r="E72" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="F72" s="47">
-        <v>3</v>
-      </c>
-      <c r="G72" s="66" t="s">
-        <v>100</v>
-      </c>
-      <c r="H72" s="50" t="s">
+      <c r="C72" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="D72" s="53">
+        <v>3600</v>
+      </c>
+      <c r="E72" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="53">
+        <v>3600</v>
+      </c>
+      <c r="G72" s="56" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="52"/>
-      <c r="B73" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="E73" s="53" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" s="53"/>
-      <c r="G73" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="H73" s="57" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="B74" s="47"/>
-      <c r="C74" s="48"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
-      <c r="F74" s="47"/>
-      <c r="G74" s="49"/>
-      <c r="H74" s="50"/>
-    </row>
-    <row r="75" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="46"/>
-      <c r="B75" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="C75" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75" s="47">
-        <v>45</v>
-      </c>
-      <c r="E75" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75" s="47">
-        <v>45</v>
-      </c>
-      <c r="G75" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="H75" s="67" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="46"/>
-      <c r="B76" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="C76" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D76" s="47">
-        <v>75</v>
-      </c>
-      <c r="E76" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F76" s="47">
-        <v>75</v>
-      </c>
-      <c r="G76" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="H76" s="67" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="18" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="46"/>
-      <c r="B77" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C77" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="D77" s="47">
-        <v>450</v>
-      </c>
-      <c r="E77" s="47" t="s">
-        <v>21</v>
-      </c>
-      <c r="F77" s="47">
-        <v>450</v>
-      </c>
-      <c r="G77" s="49" t="s">
-        <v>103</v>
-      </c>
-      <c r="H77" s="67" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" s="12" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="52"/>
-      <c r="B78" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="C78" s="54" t="s">
-        <v>1</v>
-      </c>
-      <c r="D78" s="53">
-        <v>3600</v>
-      </c>
-      <c r="E78" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="F78" s="53">
-        <v>3600</v>
-      </c>
-      <c r="G78" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="H78" s="68" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="H72" s="63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H26" r:id="rId1" xr:uid="{BFFDF1DF-AC10-154F-90C8-6E1B425878BE}"/>
-    <hyperlink ref="H31" r:id="rId2" xr:uid="{0E829C9D-F5CA-C344-BA01-6E533C5654BA}"/>
-    <hyperlink ref="H39" r:id="rId3" xr:uid="{A121E58C-073A-E143-9B04-5E9274078D9A}"/>
-    <hyperlink ref="H28" r:id="rId4" xr:uid="{B982A0B7-E477-1C4F-8364-A396A3924E00}"/>
-    <hyperlink ref="H46" r:id="rId5" xr:uid="{405EB354-6600-474D-853F-66209B7460CD}"/>
-    <hyperlink ref="H54" r:id="rId6" xr:uid="{4E8679E9-B210-6348-ADD3-3F77E2C8E25A}"/>
-    <hyperlink ref="H61" r:id="rId7" xr:uid="{8568EC0E-EC0D-F24E-843E-31850DCF03B6}"/>
-    <hyperlink ref="H64" r:id="rId8" xr:uid="{91A8231D-5654-B04D-A342-76461EC7B009}"/>
+    <hyperlink ref="H20" r:id="rId1" xr:uid="{BFFDF1DF-AC10-154F-90C8-6E1B425878BE}"/>
+    <hyperlink ref="H25" r:id="rId2" xr:uid="{0E829C9D-F5CA-C344-BA01-6E533C5654BA}"/>
+    <hyperlink ref="H33" r:id="rId3" xr:uid="{A121E58C-073A-E143-9B04-5E9274078D9A}"/>
+    <hyperlink ref="H22" r:id="rId4" xr:uid="{B982A0B7-E477-1C4F-8364-A396A3924E00}"/>
+    <hyperlink ref="H40" r:id="rId5" xr:uid="{405EB354-6600-474D-853F-66209B7460CD}"/>
+    <hyperlink ref="H48" r:id="rId6" xr:uid="{4E8679E9-B210-6348-ADD3-3F77E2C8E25A}"/>
+    <hyperlink ref="H55" r:id="rId7" xr:uid="{8568EC0E-EC0D-F24E-843E-31850DCF03B6}"/>
+    <hyperlink ref="H58" r:id="rId8" xr:uid="{91A8231D-5654-B04D-A342-76461EC7B009}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>

</xml_diff>

<commit_message>
small changes and hotfix for qrandom
</commit_message>
<xml_diff>
--- a/WF1_DevTemplate.xlsx
+++ b/WF1_DevTemplate.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C520479B-09EC-FA4C-BADF-5C05DCD015DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136BCB8F-AE40-3647-8B6A-276A0708980E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="460" windowWidth="39560" windowHeight="27560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18700" yWindow="460" windowWidth="32320" windowHeight="27540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WF1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="149">
   <si>
     <t>ExpWorkflowVer</t>
   </si>
@@ -847,6 +847,12 @@
   </si>
   <si>
     <t>['AcNH3I','GBL']</t>
+  </si>
+  <si>
+    <t>['PbI2','nDodecylammoniumIodide','GBL']</t>
+  </si>
+  <si>
+    <t>['nDodecylammoniumIodide','GBL']</t>
   </si>
 </sst>
 </file>
@@ -1540,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1549,7 +1555,7 @@
     <col min="1" max="1" width="25.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="41.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="91.5" style="5" bestFit="1" customWidth="1"/>
@@ -2009,7 +2015,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>115</v>
+        <v>145</v>
       </c>
       <c r="E24" s="35" t="s">
         <v>43</v>
@@ -2193,7 +2199,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="E32" s="35" t="s">
         <v>43</v>
@@ -2351,7 +2357,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E39" s="35" t="s">
         <v>43</v>
@@ -2531,7 +2537,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="35" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E47" s="35" t="s">
         <v>43</v>
@@ -2945,7 +2951,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="47">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E66" s="47" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
updated template; split random and specified exps
</commit_message>
<xml_diff>
--- a/WF1_DevTemplate.xlsx
+++ b/WF1_DevTemplate.xlsx
@@ -947,7 +947,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <name val="Calibri"/>
       <color rgb="FF000000"/>
@@ -1023,8 +1023,13 @@
       <sz val="11"/>
       <u val="single"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF00FFFF"/>
+      <sz val="11"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1093,8 +1098,13 @@
         <fgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border/>
     <border>
       <bottom style="thin">
@@ -1349,11 +1359,24 @@
         <color rgb="FF000000"/>
       </left>
     </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1750,6 +1773,67 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1773,7 +1857,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="topLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -2049,7 +2133,7 @@
       <c r="Y7" s="14"/>
       <c r="Z7" s="14"/>
     </row>
-    <row ht="18.75" customHeight="1" r="8" s="117" customFormat="1">
+    <row ht="18.75" customHeight="1" r="8" s="165" customFormat="1">
       <c r="A8" s="138" t="s">
         <v>30</v>
       </c>
@@ -2062,26 +2146,26 @@
         <v>31</v>
       </c>
       <c r="H8" s="142"/>
-      <c r="I8" s="143"/>
-      <c r="J8" s="143"/>
-      <c r="K8" s="143"/>
-      <c r="L8" s="143"/>
-      <c r="M8" s="143"/>
-      <c r="N8" s="143"/>
-      <c r="O8" s="143"/>
-      <c r="P8" s="143"/>
-      <c r="Q8" s="143"/>
-      <c r="R8" s="143"/>
-      <c r="S8" s="143"/>
-      <c r="T8" s="143"/>
-      <c r="U8" s="143"/>
-      <c r="V8" s="143"/>
-      <c r="W8" s="143"/>
-      <c r="X8" s="143"/>
-      <c r="Y8" s="143"/>
-      <c r="Z8" s="143"/>
-    </row>
-    <row ht="18.75" customHeight="1" r="9" s="117" customFormat="1">
+      <c r="I8" s="158"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="158"/>
+      <c r="M8" s="158"/>
+      <c r="N8" s="158"/>
+      <c r="O8" s="158"/>
+      <c r="P8" s="158"/>
+      <c r="Q8" s="158"/>
+      <c r="R8" s="158"/>
+      <c r="S8" s="158"/>
+      <c r="T8" s="158"/>
+      <c r="U8" s="158"/>
+      <c r="V8" s="158"/>
+      <c r="W8" s="158"/>
+      <c r="X8" s="158"/>
+      <c r="Y8" s="158"/>
+      <c r="Z8" s="158"/>
+    </row>
+    <row ht="18.75" customHeight="1" r="9" s="165" customFormat="1">
       <c r="A9" s="119"/>
       <c r="B9" s="120" t="s">
         <v>32</v>
@@ -2104,26 +2188,26 @@
       <c r="H9" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="123"/>
-      <c r="O9" s="123"/>
-      <c r="P9" s="123"/>
-      <c r="Q9" s="123"/>
-      <c r="R9" s="123"/>
-      <c r="S9" s="123"/>
-      <c r="T9" s="123"/>
-      <c r="U9" s="123"/>
-      <c r="V9" s="123"/>
-      <c r="W9" s="123"/>
-      <c r="X9" s="123"/>
-      <c r="Y9" s="123"/>
-      <c r="Z9" s="123"/>
-    </row>
-    <row ht="18.75" customHeight="1" r="10" s="117" customFormat="1">
+      <c r="I9" s="164"/>
+      <c r="J9" s="164"/>
+      <c r="K9" s="164"/>
+      <c r="L9" s="164"/>
+      <c r="M9" s="164"/>
+      <c r="N9" s="164"/>
+      <c r="O9" s="164"/>
+      <c r="P9" s="164"/>
+      <c r="Q9" s="164"/>
+      <c r="R9" s="164"/>
+      <c r="S9" s="164"/>
+      <c r="T9" s="164"/>
+      <c r="U9" s="164"/>
+      <c r="V9" s="164"/>
+      <c r="W9" s="164"/>
+      <c r="X9" s="164"/>
+      <c r="Y9" s="164"/>
+      <c r="Z9" s="164"/>
+    </row>
+    <row ht="18.75" customHeight="1" r="10" s="165" customFormat="1">
       <c r="A10" s="119"/>
       <c r="B10" s="120" t="s">
         <v>38</v>
@@ -2144,26 +2228,26 @@
       <c r="H10" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="123"/>
-      <c r="J10" s="123"/>
-      <c r="K10" s="123"/>
-      <c r="L10" s="123"/>
-      <c r="M10" s="123"/>
-      <c r="N10" s="123"/>
-      <c r="O10" s="123"/>
-      <c r="P10" s="123"/>
-      <c r="Q10" s="123"/>
-      <c r="R10" s="123"/>
-      <c r="S10" s="123"/>
-      <c r="T10" s="123"/>
-      <c r="U10" s="123"/>
-      <c r="V10" s="123"/>
-      <c r="W10" s="123"/>
-      <c r="X10" s="123"/>
-      <c r="Y10" s="123"/>
-      <c r="Z10" s="123"/>
-    </row>
-    <row ht="18.75" customHeight="1" r="11" s="117" customFormat="1">
+      <c r="I10" s="164"/>
+      <c r="J10" s="164"/>
+      <c r="K10" s="164"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="164"/>
+      <c r="N10" s="164"/>
+      <c r="O10" s="164"/>
+      <c r="P10" s="164"/>
+      <c r="Q10" s="164"/>
+      <c r="R10" s="164"/>
+      <c r="S10" s="164"/>
+      <c r="T10" s="164"/>
+      <c r="U10" s="164"/>
+      <c r="V10" s="164"/>
+      <c r="W10" s="164"/>
+      <c r="X10" s="164"/>
+      <c r="Y10" s="164"/>
+      <c r="Z10" s="164"/>
+    </row>
+    <row ht="18.95" customHeight="1" r="11" s="165" customFormat="1">
       <c r="A11" s="119"/>
       <c r="B11" s="120" t="s">
         <v>42</v>
@@ -2172,7 +2256,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="120">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E11" s="120" t="s">
         <v>21</v>
@@ -2184,24 +2268,24 @@
       <c r="H11" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="123"/>
-      <c r="N11" s="123"/>
-      <c r="O11" s="123"/>
-      <c r="P11" s="123"/>
-      <c r="Q11" s="123"/>
-      <c r="R11" s="123"/>
-      <c r="S11" s="123"/>
-      <c r="T11" s="123"/>
-      <c r="U11" s="123"/>
-      <c r="V11" s="123"/>
-      <c r="W11" s="123"/>
-      <c r="X11" s="123"/>
-      <c r="Y11" s="123"/>
-      <c r="Z11" s="123"/>
+      <c r="I11" s="164"/>
+      <c r="J11" s="164"/>
+      <c r="K11" s="164"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="164"/>
+      <c r="N11" s="164"/>
+      <c r="O11" s="164"/>
+      <c r="P11" s="164"/>
+      <c r="Q11" s="164"/>
+      <c r="R11" s="164"/>
+      <c r="S11" s="164"/>
+      <c r="T11" s="164"/>
+      <c r="U11" s="164"/>
+      <c r="V11" s="164"/>
+      <c r="W11" s="164"/>
+      <c r="X11" s="164"/>
+      <c r="Y11" s="164"/>
+      <c r="Z11" s="164"/>
     </row>
     <row ht="18.75" customHeight="1" r="12">
       <c r="A12" s="119"/>
@@ -2288,13 +2372,13 @@
         <v>10</v>
       </c>
       <c r="D14" s="120">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="E14" s="120" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="120"/>
-      <c r="G14" s="123" t="s">
+      <c r="F14" s="147"/>
+      <c r="G14" s="121" t="s">
         <v>43</v>
       </c>
       <c r="H14" s="123"/>
@@ -2318,18 +2402,35 @@
       <c r="Z14" s="14"/>
     </row>
     <row r="15">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="146" t="s">
         <v>49</v>
       </c>
+      <c r="B15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="117"/>
+      <c r="E15" s="117"/>
+      <c r="F15" s="148"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="117"/>
     </row>
     <row r="16">
-      <c r="B16" s="0" t="s">
+      <c r="A16" s="149"/>
+      <c r="B16" s="149" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="120">
+      <c r="C16" s="149"/>
+      <c r="D16" s="150">
         <f>D7-D11-D14</f>
-        <v>46</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E16" s="149" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="166">
+        <v>2</v>
+      </c>
+      <c r="G16" s="168"/>
+      <c r="H16" s="149"/>
     </row>
     <row ht="18.75" customHeight="1" r="17">
       <c r="A17" s="63" t="s">
@@ -13872,7 +13973,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -13884,336 +13985,333 @@
       <c r="A1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>167</v>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="120">
+        <f>WF1!D11+WF1!D14+1</f>
+        <v>96</v>
+      </c>
+      <c r="B2" s="0">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="0">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D2" s="0">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="0">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F2" s="0">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G2" s="0">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H2" s="0">
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="0">
-        <f>WF1!D11+WF1!D14+1</f>
-        <v>51</v>
-      </c>
-      <c r="C2" s="0">
-        <v>1</v>
-      </c>
-      <c r="D2" s="0">
-        <v>2</v>
-      </c>
-      <c r="E2" s="0">
-        <v>3</v>
-      </c>
-      <c r="F2" s="0">
-        <v>45</v>
-      </c>
-      <c r="G2" s="0">
-        <v>2381</v>
-      </c>
-      <c r="H2" s="0">
-        <v>6</v>
-      </c>
-      <c r="I2" s="0">
-        <v>7</v>
-      </c>
-    </row>
     <row r="3">
-      <c r="A3" s="0">
+      <c r="A3" s="120" t="str">
         <f>IF(A2&lt;wellcount,A2+1,"")</f>
-        <v>52</v>
+        <v/>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0">
+      <c r="A4" s="120" t="str">
         <f>IF(A3&lt;wellcount,A3+1,"")</f>
-        <v>53</v>
+        <v/>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0">
+      <c r="A5" s="120" t="str">
         <f>IF(A4&lt;wellcount,A4+1,"")</f>
-        <v>54</v>
+        <v/>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0">
+      <c r="A6" s="120" t="str">
         <f>IF(A5&lt;wellcount,A5+1,"")</f>
-        <v>55</v>
+        <v/>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0">
+      <c r="A7" s="120" t="str">
         <f>IF(A6&lt;wellcount,A6+1,"")</f>
-        <v>56</v>
+        <v/>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0">
+      <c r="A8" s="120" t="str">
         <f>IF(A7&lt;wellcount,A7+1,"")</f>
-        <v>57</v>
+        <v/>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="0">
+      <c r="A9" s="120" t="str">
         <f>IF(A8&lt;wellcount,A8+1,"")</f>
-        <v>58</v>
+        <v/>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="0">
+      <c r="A10" s="120" t="str">
         <f>IF(A9&lt;wellcount,A9+1,"")</f>
-        <v>59</v>
+        <v/>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="0">
+      <c r="A11" s="120" t="str">
         <f>IF(A10&lt;wellcount,A10+1,"")</f>
-        <v>60</v>
+        <v/>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="0">
+      <c r="A12" s="120" t="str">
         <f>IF(A11&lt;wellcount,A11+1,"")</f>
-        <v>61</v>
+        <v/>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="0">
+      <c r="A13" s="120" t="str">
         <f>IF(A12&lt;wellcount,A12+1,"")</f>
-        <v>62</v>
+        <v/>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
+      <c r="A14" s="120" t="str">
         <f>IF(A13&lt;wellcount,A13+1,"")</f>
-        <v>63</v>
+        <v/>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="0">
+      <c r="A15" s="120" t="str">
         <f>IF(A14&lt;wellcount,A14+1,"")</f>
-        <v>64</v>
+        <v/>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="0">
+      <c r="A16" s="120" t="str">
         <f>IF(A15&lt;wellcount,A15+1,"")</f>
-        <v>65</v>
+        <v/>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="0">
+      <c r="A17" s="120" t="str">
         <f>IF(A16&lt;wellcount,A16+1,"")</f>
-        <v>66</v>
+        <v/>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="0">
+      <c r="A18" s="120" t="str">
         <f>IF(A17&lt;wellcount,A17+1,"")</f>
-        <v>67</v>
+        <v/>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="0">
+      <c r="A19" s="120" t="str">
         <f>IF(A18&lt;wellcount,A18+1,"")</f>
-        <v>68</v>
+        <v/>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="0">
+      <c r="A20" s="120" t="str">
         <f>IF(A19&lt;wellcount,A19+1,"")</f>
-        <v>69</v>
+        <v/>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="0">
+      <c r="A21" s="120" t="str">
         <f>IF(A20&lt;wellcount,A20+1,"")</f>
-        <v>70</v>
+        <v/>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="0">
+      <c r="A22" s="120" t="str">
         <f>IF(A21&lt;wellcount,A21+1,"")</f>
-        <v>71</v>
+        <v/>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="0">
+      <c r="A23" s="120" t="str">
         <f>IF(A22&lt;wellcount,A22+1,"")</f>
-        <v>72</v>
+        <v/>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="0">
+      <c r="A24" s="120" t="str">
         <f>IF(A23&lt;wellcount,A23+1,"")</f>
-        <v>73</v>
+        <v/>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="0">
+      <c r="A25" s="120" t="str">
         <f>IF(A24&lt;wellcount,A24+1,"")</f>
-        <v>74</v>
+        <v/>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="0">
+      <c r="A26" s="120" t="str">
         <f>IF(A25&lt;wellcount,A25+1,"")</f>
-        <v>75</v>
+        <v/>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="0">
+      <c r="A27" s="120" t="str">
         <f>IF(A26&lt;wellcount,A26+1,"")</f>
-        <v>76</v>
+        <v/>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="0">
+      <c r="A28" s="120" t="str">
         <f>IF(A27&lt;wellcount,A27+1,"")</f>
-        <v>77</v>
+        <v/>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="0">
+      <c r="A29" s="120" t="str">
         <f>IF(A28&lt;wellcount,A28+1,"")</f>
-        <v>78</v>
+        <v/>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="0">
+      <c r="A30" s="120" t="str">
         <f>IF(A29&lt;wellcount,A29+1,"")</f>
-        <v>79</v>
+        <v/>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="0">
+      <c r="A31" s="120" t="str">
         <f>IF(A30&lt;wellcount,A30+1,"")</f>
-        <v>80</v>
+        <v/>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="0">
+      <c r="A32" s="120" t="str">
         <f>IF(A31&lt;wellcount,A31+1,"")</f>
-        <v>81</v>
+        <v/>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="0">
+      <c r="A33" s="120" t="str">
         <f>IF(A32&lt;wellcount,A32+1,"")</f>
-        <v>82</v>
+        <v/>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="0">
+      <c r="A34" s="120" t="str">
         <f>IF(A33&lt;wellcount,A33+1,"")</f>
-        <v>83</v>
+        <v/>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="0">
+      <c r="A35" s="120" t="str">
         <f>IF(A34&lt;wellcount,A34+1,"")</f>
-        <v>84</v>
+        <v/>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="0">
+      <c r="A36" s="120" t="str">
         <f>IF(A35&lt;wellcount,A35+1,"")</f>
-        <v>85</v>
+        <v/>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="0">
+      <c r="A37" s="120" t="str">
         <f>IF(A36&lt;wellcount,A36+1,"")</f>
-        <v>86</v>
+        <v/>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="0">
+      <c r="A38" s="120" t="str">
         <f>IF(A37&lt;wellcount,A37+1,"")</f>
-        <v>87</v>
+        <v/>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="0">
+      <c r="A39" s="120" t="str">
         <f>IF(A38&lt;wellcount,A38+1,"")</f>
-        <v>88</v>
+        <v/>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="0">
+      <c r="A40" s="120" t="str">
         <f>IF(A39&lt;wellcount,A39+1,"")</f>
-        <v>89</v>
+        <v/>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="0">
+      <c r="A41" s="120" t="str">
         <f>IF(A40&lt;wellcount,A40+1,"")</f>
-        <v>90</v>
+        <v/>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="0">
+      <c r="A42" s="120" t="str">
         <f>IF(A41&lt;wellcount,A41+1,"")</f>
-        <v>91</v>
+        <v/>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="0">
+      <c r="A43" s="120" t="str">
         <f>IF(A42&lt;wellcount,A42+1,"")</f>
-        <v>92</v>
+        <v/>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="0">
+      <c r="A44" s="120" t="str">
         <f>IF(A43&lt;wellcount,A43+1,"")</f>
-        <v>93</v>
+        <v/>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="0">
+      <c r="A45" s="120" t="str">
         <f>IF(A44&lt;wellcount,A44+1,"")</f>
-        <v>94</v>
+        <v/>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="0">
+      <c r="A46" s="120" t="str">
         <f>IF(A45&lt;wellcount,A45+1,"")</f>
-        <v>95</v>
+        <v/>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="0">
+      <c r="A47" s="120" t="str">
         <f>IF(A46&lt;wellcount,A46+1,"")</f>
-        <v>96</v>
+        <v/>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="str">
+      <c r="A48" s="120" t="str">
         <f>IF(A47&lt;wellcount,A47+1,"")</f>
         <v/>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="str">
+      <c r="A49" s="120" t="str">
         <f>IF(A48&lt;wellcount,A48+1,"")</f>
         <v/>
       </c>

</xml_diff>

<commit_message>
* add total volume column in ManualExps sheet * cleanup UI:     * Manual Exp well numbers only appear if manual_exps > 0:         * (see ManualExps!A2)     * Update validation statement for well_count
</commit_message>
<xml_diff>
--- a/WF1_DevTemplate.xlsx
+++ b/WF1_DevTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="380" windowWidth="25600" windowHeight="15620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WF1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
   </sheets>
   <definedNames>
     <definedName name="fixed_wells">'WF1'!$D$16</definedName>
+    <definedName name="manual_wells">'WF1'!$D$16</definedName>
     <definedName name="wellcount">'WF1'!$D$7</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="168">
   <si>
     <t>Reagent1 (ul)</t>
   </si>
@@ -920,10 +921,13 @@
     <t>manual_wells</t>
   </si>
   <si>
-    <t>WF1 max = 96   (all exp&lt;index&gt;_wells and manual_wells variables MUST sum to this value)</t>
-  </si>
-  <si>
     <t>Manual Well Number</t>
+  </si>
+  <si>
+    <t>WF1 max = 96   (all exp&lt;index&gt;_wells and manual_wells MUST sum to this value)</t>
+  </si>
+  <si>
+    <t>Total Volume</t>
   </si>
 </sst>
 </file>
@@ -1315,7 +1319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1595,6 +1599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1875,7 +1880,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2131,7 +2136,7 @@
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="24" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H7" s="25"/>
       <c r="I7" s="14"/>
@@ -2438,7 +2443,9 @@
       <c r="B16" s="91" t="s">
         <v>164</v>
       </c>
-      <c r="C16" s="91"/>
+      <c r="C16" s="91" t="s">
+        <v>9</v>
+      </c>
       <c r="D16" s="92">
         <v>0</v>
       </c>
@@ -13973,9 +13980,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="wellcount" prompt="MUST be sum of random_wellcount and fixed_wells" sqref="D7">
-      <formula1>SUM(#REF!,D16)</formula1>
-    </dataValidation>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="wellcount" prompt="MUST be sum of exp&lt;index&gt;_wells and manual_wells" sqref="D7"/>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="H19" r:id="rId1"/>
@@ -13995,20 +14000,21 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H500"/>
+  <dimension ref="A1:I500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="101"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="100" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="100" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -14031,1790 +14037,2581 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="101" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="99" t="str">
+        <f>IF(fixed_wells &gt; 0, 1, "")</f>
+        <v/>
+      </c>
+      <c r="I2" s="101" t="str">
+        <f>IF(NOT(A2 = ""), SUM(B2:H2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="99" t="str">
-        <f>IF(A2 &lt; fixed_wells, A2 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="A3:A34" si="0">IF(A2 &lt; fixed_wells, A2 + 1, "")</f>
+        <v/>
+      </c>
+      <c r="I3" s="101" t="str">
+        <f t="shared" ref="I3:I66" si="1">IF(NOT(A3 = ""), SUM(B3:H3), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="str">
-        <f>IF(A3 &lt; fixed_wells, A3 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I4" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="99" t="str">
-        <f>IF(A4 &lt; fixed_wells, A4 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I5" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="99" t="str">
-        <f>IF(A5 &lt; fixed_wells, A5 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I6" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="99" t="str">
-        <f>IF(A6 &lt; fixed_wells, A6 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I7" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="str">
-        <f>IF(A7 &lt; fixed_wells, A7 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I8" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="99" t="str">
-        <f>IF(A8 &lt; fixed_wells, A8 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I9" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="99" t="str">
-        <f>IF(A9 &lt; fixed_wells, A9 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I10" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="99" t="str">
-        <f>IF(A10 &lt; fixed_wells, A10 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I11" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="99" t="str">
-        <f>IF(A11 &lt; fixed_wells, A11 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I12" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="99" t="str">
-        <f>IF(A12 &lt; fixed_wells, A12 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I13" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="99" t="str">
-        <f>IF(A13 &lt; fixed_wells, A13 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I14" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="99" t="str">
-        <f>IF(A14 &lt; fixed_wells, A14 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I15" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="99" t="str">
-        <f>IF(A15 &lt; fixed_wells, A15 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I16" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="99" t="str">
-        <f>IF(A16 &lt; fixed_wells, A16 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I17" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="99" t="str">
-        <f>IF(A17 &lt; fixed_wells, A17 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I18" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="99" t="str">
-        <f>IF(A18 &lt; fixed_wells, A18 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I19" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="99" t="str">
-        <f>IF(A19 &lt; fixed_wells, A19 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I20" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="99" t="str">
-        <f>IF(A20 &lt; fixed_wells, A20 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I21" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="99" t="str">
-        <f>IF(A21 &lt; fixed_wells, A21 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I22" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="99" t="str">
-        <f>IF(A22 &lt; fixed_wells, A22 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I23" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="99" t="str">
-        <f>IF(A23 &lt; fixed_wells, A23 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I24" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="99" t="str">
-        <f>IF(A24 &lt; fixed_wells, A24 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I25" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="99" t="str">
-        <f>IF(A25 &lt; fixed_wells, A25 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I26" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="99" t="str">
-        <f>IF(A26 &lt; fixed_wells, A26 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I27" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="99" t="str">
-        <f>IF(A27 &lt; fixed_wells, A27 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I28" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="99" t="str">
-        <f>IF(A28 &lt; fixed_wells, A28 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="30" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I29" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="99" t="str">
-        <f>IF(A29 &lt; fixed_wells, A29 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I30" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="99" t="str">
-        <f>IF(A30 &lt; fixed_wells, A30 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I31" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="99" t="str">
-        <f>IF(A31 &lt; fixed_wells, A31 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I32" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="99" t="str">
-        <f>IF(A32 &lt; fixed_wells, A32 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I33" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="99" t="str">
-        <f>IF(A33 &lt; fixed_wells, A33 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I34" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="99" t="str">
-        <f>IF(A34 &lt; fixed_wells, A34 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="A35:A66" si="2">IF(A34 &lt; fixed_wells, A34 + 1, "")</f>
+        <v/>
+      </c>
+      <c r="I35" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="99" t="str">
-        <f>IF(A35 &lt; fixed_wells, A35 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I36" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="99" t="str">
-        <f>IF(A36 &lt; fixed_wells, A36 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I37" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="99" t="str">
-        <f>IF(A37 &lt; fixed_wells, A37 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I38" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="99" t="str">
-        <f>IF(A38 &lt; fixed_wells, A38 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I39" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="99" t="str">
-        <f>IF(A39 &lt; fixed_wells, A39 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I40" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="99" t="str">
-        <f>IF(A40 &lt; fixed_wells, A40 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I41" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="99" t="str">
-        <f>IF(A41 &lt; fixed_wells, A41 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I42" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="99" t="str">
-        <f>IF(A42 &lt; fixed_wells, A42 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I43" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="99" t="str">
-        <f>IF(A43 &lt; fixed_wells, A43 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I44" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="99" t="str">
-        <f>IF(A44 &lt; fixed_wells, A44 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I45" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="99" t="str">
-        <f>IF(A45 &lt; fixed_wells, A45 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I46" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="99" t="str">
-        <f>IF(A46 &lt; fixed_wells, A46 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I47" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="99" t="str">
-        <f>IF(A47 &lt; fixed_wells, A47 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I48" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="99" t="str">
-        <f>IF(A48 &lt; fixed_wells, A48 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I49" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="99" t="str">
-        <f>IF(A49 &lt; fixed_wells, A49 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I50" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="99" t="str">
-        <f>IF(A50 &lt; fixed_wells, A50 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I51" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="99" t="str">
-        <f>IF(A51 &lt; fixed_wells, A51 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I52" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="99" t="str">
-        <f>IF(A52 &lt; fixed_wells, A52 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I53" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="99" t="str">
-        <f>IF(A53 &lt; fixed_wells, A53 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I54" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="99" t="str">
-        <f>IF(A54 &lt; fixed_wells, A54 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I55" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="99" t="str">
-        <f>IF(A55 &lt; fixed_wells, A55 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="57" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I56" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="99" t="str">
-        <f>IF(A56 &lt; fixed_wells, A56 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I57" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="99" t="str">
-        <f>IF(A57 &lt; fixed_wells, A57 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I58" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="99" t="str">
-        <f>IF(A58 &lt; fixed_wells, A58 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I59" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="99" t="str">
-        <f>IF(A59 &lt; fixed_wells, A59 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I60" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="99" t="str">
-        <f>IF(A60 &lt; fixed_wells, A60 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I61" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="99" t="str">
-        <f>IF(A61 &lt; fixed_wells, A61 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I62" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="99" t="str">
-        <f>IF(A62 &lt; fixed_wells, A62 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I63" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="99" t="str">
-        <f>IF(A63 &lt; fixed_wells, A63 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="65" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I64" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="99" t="str">
-        <f>IF(A64 &lt; fixed_wells, A64 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I65" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="99" t="str">
-        <f>IF(A65 &lt; fixed_wells, A65 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="67" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I66" s="101" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="99" t="str">
-        <f>IF(A66 &lt; fixed_wells, A66 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="A67:A97" si="3">IF(A66 &lt; fixed_wells, A66 + 1, "")</f>
+        <v/>
+      </c>
+      <c r="I67" s="101" t="str">
+        <f t="shared" ref="I67:I97" si="4">IF(NOT(A67 = ""), SUM(B67:H67), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="99" t="str">
-        <f>IF(A67 &lt; fixed_wells, A67 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I68" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="str">
-        <f>IF(A68 &lt; fixed_wells, A68 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I69" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="99" t="str">
-        <f>IF(A69 &lt; fixed_wells, A69 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I70" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="99" t="str">
-        <f>IF(A70 &lt; fixed_wells, A70 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I71" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="99" t="str">
-        <f>IF(A71 &lt; fixed_wells, A71 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I72" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="99" t="str">
-        <f>IF(A72 &lt; fixed_wells, A72 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="74" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I73" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="99" t="str">
-        <f>IF(A73 &lt; fixed_wells, A73 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I74" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="99" t="str">
-        <f>IF(A74 &lt; fixed_wells, A74 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I75" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="99" t="str">
-        <f>IF(A75 &lt; fixed_wells, A75 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I76" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="99" t="str">
-        <f>IF(A76 &lt; fixed_wells, A76 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="78" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I77" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="99" t="str">
-        <f>IF(A77 &lt; fixed_wells, A77 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="79" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I78" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="99" t="str">
-        <f>IF(A78 &lt; fixed_wells, A78 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="80" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I79" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="99" t="str">
-        <f>IF(A79 &lt; fixed_wells, A79 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="81" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I80" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="99" t="str">
-        <f>IF(A80 &lt; fixed_wells, A80 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="82" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I81" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="99" t="str">
-        <f>IF(A81 &lt; fixed_wells, A81 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="83" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I82" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="99" t="str">
-        <f>IF(A82 &lt; fixed_wells, A82 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="84" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I83" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="99" t="str">
-        <f>IF(A83 &lt; fixed_wells, A83 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I84" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="99" t="str">
-        <f>IF(A84 &lt; fixed_wells, A84 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="86" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I85" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="99" t="str">
-        <f>IF(A85 &lt; fixed_wells, A85 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="87" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I86" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="99" t="str">
-        <f>IF(A86 &lt; fixed_wells, A86 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="88" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I87" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="99" t="str">
-        <f>IF(A87 &lt; fixed_wells, A87 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I88" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="99" t="str">
-        <f>IF(A88 &lt; fixed_wells, A88 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="90" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I89" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="99" t="str">
-        <f>IF(A89 &lt; fixed_wells, A89 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I90" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="99" t="str">
-        <f>IF(A90 &lt; fixed_wells, A90 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="92" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I91" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="99" t="str">
-        <f>IF(A91 &lt; fixed_wells, A91 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I92" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="93" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="99" t="str">
-        <f>IF(A92 &lt; fixed_wells, A92 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="94" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I93" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="94" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="99" t="str">
-        <f>IF(A93 &lt; fixed_wells, A93 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="95" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I94" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="95" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="99" t="str">
-        <f>IF(A94 &lt; fixed_wells, A94 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="96" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I95" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="96" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="99" t="str">
-        <f>IF(A95 &lt; fixed_wells, A95 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I96" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="99" t="str">
-        <f>IF(A96 &lt; fixed_wells, A96 + 1, "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="98" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="I97" s="101" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98"/>
-    </row>
-    <row r="99" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I98" s="101"/>
+    </row>
+    <row r="99" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99"/>
-    </row>
-    <row r="100" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I99" s="101"/>
+    </row>
+    <row r="100" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100"/>
-    </row>
-    <row r="101" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I100" s="101"/>
+    </row>
+    <row r="101" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101"/>
-    </row>
-    <row r="102" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I101" s="101"/>
+    </row>
+    <row r="102" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102"/>
-    </row>
-    <row r="103" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I102" s="101"/>
+    </row>
+    <row r="103" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103"/>
-    </row>
-    <row r="104" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I103" s="101"/>
+    </row>
+    <row r="104" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104"/>
-    </row>
-    <row r="105" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I104" s="101"/>
+    </row>
+    <row r="105" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105"/>
-    </row>
-    <row r="106" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I105" s="101"/>
+    </row>
+    <row r="106" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A106"/>
-    </row>
-    <row r="107" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I106" s="101"/>
+    </row>
+    <row r="107" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A107"/>
-    </row>
-    <row r="108" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I107" s="101"/>
+    </row>
+    <row r="108" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A108"/>
-    </row>
-    <row r="109" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I108" s="101"/>
+    </row>
+    <row r="109" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A109"/>
-    </row>
-    <row r="110" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I109" s="101"/>
+    </row>
+    <row r="110" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110"/>
-    </row>
-    <row r="111" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I110" s="101"/>
+    </row>
+    <row r="111" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111"/>
-    </row>
-    <row r="112" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I111" s="101"/>
+    </row>
+    <row r="112" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A112"/>
-    </row>
-    <row r="113" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I112" s="101"/>
+    </row>
+    <row r="113" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A113"/>
-    </row>
-    <row r="114" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I113" s="101"/>
+    </row>
+    <row r="114" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A114"/>
-    </row>
-    <row r="115" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I114" s="101"/>
+    </row>
+    <row r="115" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A115"/>
-    </row>
-    <row r="116" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I115" s="101"/>
+    </row>
+    <row r="116" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A116"/>
-    </row>
-    <row r="117" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I116" s="101"/>
+    </row>
+    <row r="117" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A117"/>
-    </row>
-    <row r="118" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I117" s="101"/>
+    </row>
+    <row r="118" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A118"/>
-    </row>
-    <row r="119" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I118" s="101"/>
+    </row>
+    <row r="119" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A119"/>
-    </row>
-    <row r="120" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I119" s="101"/>
+    </row>
+    <row r="120" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A120"/>
-    </row>
-    <row r="121" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I120" s="101"/>
+    </row>
+    <row r="121" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A121"/>
-    </row>
-    <row r="122" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I121" s="101"/>
+    </row>
+    <row r="122" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A122"/>
-    </row>
-    <row r="123" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I122" s="101"/>
+    </row>
+    <row r="123" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A123"/>
-    </row>
-    <row r="124" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I123" s="101"/>
+    </row>
+    <row r="124" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A124"/>
-    </row>
-    <row r="125" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I124" s="101"/>
+    </row>
+    <row r="125" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A125"/>
-    </row>
-    <row r="126" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I125" s="101"/>
+    </row>
+    <row r="126" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A126"/>
-    </row>
-    <row r="127" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I126" s="101"/>
+    </row>
+    <row r="127" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A127"/>
-    </row>
-    <row r="128" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I127" s="101"/>
+    </row>
+    <row r="128" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A128"/>
-    </row>
-    <row r="129" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I128" s="101"/>
+    </row>
+    <row r="129" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A129"/>
-    </row>
-    <row r="130" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I129" s="101"/>
+    </row>
+    <row r="130" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A130"/>
-    </row>
-    <row r="131" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I130" s="101"/>
+    </row>
+    <row r="131" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A131"/>
-    </row>
-    <row r="132" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I131" s="101"/>
+    </row>
+    <row r="132" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A132"/>
-    </row>
-    <row r="133" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I132" s="101"/>
+    </row>
+    <row r="133" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A133"/>
-    </row>
-    <row r="134" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I133" s="101"/>
+    </row>
+    <row r="134" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A134"/>
-    </row>
-    <row r="135" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I134" s="101"/>
+    </row>
+    <row r="135" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A135"/>
-    </row>
-    <row r="136" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I135" s="101"/>
+    </row>
+    <row r="136" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A136"/>
-    </row>
-    <row r="137" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I136" s="101"/>
+    </row>
+    <row r="137" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137"/>
-    </row>
-    <row r="138" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I137" s="101"/>
+    </row>
+    <row r="138" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138"/>
-    </row>
-    <row r="139" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I138" s="101"/>
+    </row>
+    <row r="139" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139"/>
-    </row>
-    <row r="140" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I139" s="101"/>
+    </row>
+    <row r="140" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A140"/>
-    </row>
-    <row r="141" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I140" s="101"/>
+    </row>
+    <row r="141" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A141"/>
-    </row>
-    <row r="142" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I141" s="101"/>
+    </row>
+    <row r="142" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A142"/>
-    </row>
-    <row r="143" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I142" s="101"/>
+    </row>
+    <row r="143" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A143"/>
-    </row>
-    <row r="144" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I143" s="101"/>
+    </row>
+    <row r="144" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A144"/>
-    </row>
-    <row r="145" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I144" s="101"/>
+    </row>
+    <row r="145" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A145"/>
-    </row>
-    <row r="146" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I145" s="101"/>
+    </row>
+    <row r="146" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A146"/>
-    </row>
-    <row r="147" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I146" s="101"/>
+    </row>
+    <row r="147" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A147"/>
-    </row>
-    <row r="148" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I147" s="101"/>
+    </row>
+    <row r="148" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A148"/>
-    </row>
-    <row r="149" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I148" s="101"/>
+    </row>
+    <row r="149" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A149"/>
-    </row>
-    <row r="150" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I149" s="101"/>
+    </row>
+    <row r="150" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A150"/>
-    </row>
-    <row r="151" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I150" s="101"/>
+    </row>
+    <row r="151" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A151"/>
-    </row>
-    <row r="152" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I151" s="101"/>
+    </row>
+    <row r="152" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A152"/>
-    </row>
-    <row r="153" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I152" s="101"/>
+    </row>
+    <row r="153" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A153"/>
-    </row>
-    <row r="154" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I153" s="101"/>
+    </row>
+    <row r="154" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A154"/>
-    </row>
-    <row r="155" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I154" s="101"/>
+    </row>
+    <row r="155" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A155"/>
-    </row>
-    <row r="156" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I155" s="101"/>
+    </row>
+    <row r="156" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A156"/>
-    </row>
-    <row r="157" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I156" s="101"/>
+    </row>
+    <row r="157" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A157"/>
-    </row>
-    <row r="158" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I157" s="101"/>
+    </row>
+    <row r="158" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A158"/>
-    </row>
-    <row r="159" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I158" s="101"/>
+    </row>
+    <row r="159" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A159"/>
-    </row>
-    <row r="160" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I159" s="101"/>
+    </row>
+    <row r="160" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A160"/>
-    </row>
-    <row r="161" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I160" s="101"/>
+    </row>
+    <row r="161" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A161"/>
-    </row>
-    <row r="162" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I161" s="101"/>
+    </row>
+    <row r="162" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A162"/>
-    </row>
-    <row r="163" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I162" s="101"/>
+    </row>
+    <row r="163" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A163"/>
-    </row>
-    <row r="164" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I163" s="101"/>
+    </row>
+    <row r="164" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A164"/>
-    </row>
-    <row r="165" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I164" s="101"/>
+    </row>
+    <row r="165" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A165"/>
-    </row>
-    <row r="166" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I165" s="101"/>
+    </row>
+    <row r="166" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A166"/>
-    </row>
-    <row r="167" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I166" s="101"/>
+    </row>
+    <row r="167" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A167"/>
-    </row>
-    <row r="168" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I167" s="101"/>
+    </row>
+    <row r="168" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A168"/>
-    </row>
-    <row r="169" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I168" s="101"/>
+    </row>
+    <row r="169" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A169"/>
-    </row>
-    <row r="170" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I169" s="101"/>
+    </row>
+    <row r="170" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A170"/>
-    </row>
-    <row r="171" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I170" s="101"/>
+    </row>
+    <row r="171" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A171"/>
-    </row>
-    <row r="172" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I171" s="101"/>
+    </row>
+    <row r="172" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A172"/>
-    </row>
-    <row r="173" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I172" s="101"/>
+    </row>
+    <row r="173" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A173"/>
-    </row>
-    <row r="174" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I173" s="101"/>
+    </row>
+    <row r="174" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A174"/>
-    </row>
-    <row r="175" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I174" s="101"/>
+    </row>
+    <row r="175" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A175"/>
-    </row>
-    <row r="176" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I175" s="101"/>
+    </row>
+    <row r="176" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A176"/>
-    </row>
-    <row r="177" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I176" s="101"/>
+    </row>
+    <row r="177" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A177"/>
-    </row>
-    <row r="178" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I177" s="101"/>
+    </row>
+    <row r="178" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A178"/>
-    </row>
-    <row r="179" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I178" s="101"/>
+    </row>
+    <row r="179" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A179"/>
-    </row>
-    <row r="180" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I179" s="101"/>
+    </row>
+    <row r="180" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A180"/>
-    </row>
-    <row r="181" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I180" s="101"/>
+    </row>
+    <row r="181" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A181"/>
-    </row>
-    <row r="182" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I181" s="101"/>
+    </row>
+    <row r="182" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A182"/>
-    </row>
-    <row r="183" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I182" s="101"/>
+    </row>
+    <row r="183" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A183"/>
-    </row>
-    <row r="184" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I183" s="101"/>
+    </row>
+    <row r="184" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A184"/>
-    </row>
-    <row r="185" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I184" s="101"/>
+    </row>
+    <row r="185" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A185"/>
-    </row>
-    <row r="186" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I185" s="101"/>
+    </row>
+    <row r="186" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A186"/>
-    </row>
-    <row r="187" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I186" s="101"/>
+    </row>
+    <row r="187" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A187"/>
-    </row>
-    <row r="188" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I187" s="101"/>
+    </row>
+    <row r="188" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A188"/>
-    </row>
-    <row r="189" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I188" s="101"/>
+    </row>
+    <row r="189" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A189"/>
-    </row>
-    <row r="190" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I189" s="101"/>
+    </row>
+    <row r="190" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A190"/>
-    </row>
-    <row r="191" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I190" s="101"/>
+    </row>
+    <row r="191" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A191"/>
-    </row>
-    <row r="192" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I191" s="101"/>
+    </row>
+    <row r="192" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A192"/>
-    </row>
-    <row r="193" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I192" s="101"/>
+    </row>
+    <row r="193" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A193"/>
-    </row>
-    <row r="194" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I193" s="101"/>
+    </row>
+    <row r="194" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A194"/>
-    </row>
-    <row r="195" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I194" s="101"/>
+    </row>
+    <row r="195" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A195"/>
-    </row>
-    <row r="196" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I195" s="101"/>
+    </row>
+    <row r="196" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A196"/>
-    </row>
-    <row r="197" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I196" s="101"/>
+    </row>
+    <row r="197" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A197"/>
-    </row>
-    <row r="198" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I197" s="101"/>
+    </row>
+    <row r="198" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198"/>
-    </row>
-    <row r="199" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I198" s="101"/>
+    </row>
+    <row r="199" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A199"/>
-    </row>
-    <row r="200" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I199" s="101"/>
+    </row>
+    <row r="200" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A200"/>
-    </row>
-    <row r="201" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I200" s="101"/>
+    </row>
+    <row r="201" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201"/>
-    </row>
-    <row r="202" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I201" s="101"/>
+    </row>
+    <row r="202" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202"/>
-    </row>
-    <row r="203" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I202" s="101"/>
+    </row>
+    <row r="203" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203"/>
-    </row>
-    <row r="204" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I203" s="101"/>
+    </row>
+    <row r="204" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204"/>
-    </row>
-    <row r="205" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I204" s="101"/>
+    </row>
+    <row r="205" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205"/>
-    </row>
-    <row r="206" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I205" s="101"/>
+    </row>
+    <row r="206" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206"/>
-    </row>
-    <row r="207" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I206" s="101"/>
+    </row>
+    <row r="207" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207"/>
-    </row>
-    <row r="208" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I207" s="101"/>
+    </row>
+    <row r="208" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A208"/>
-    </row>
-    <row r="209" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I208" s="101"/>
+    </row>
+    <row r="209" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A209"/>
-    </row>
-    <row r="210" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I209" s="101"/>
+    </row>
+    <row r="210" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A210"/>
-    </row>
-    <row r="211" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I210" s="101"/>
+    </row>
+    <row r="211" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A211"/>
-    </row>
-    <row r="212" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I211" s="101"/>
+    </row>
+    <row r="212" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A212"/>
-    </row>
-    <row r="213" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I212" s="101"/>
+    </row>
+    <row r="213" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A213"/>
-    </row>
-    <row r="214" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I213" s="101"/>
+    </row>
+    <row r="214" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A214"/>
-    </row>
-    <row r="215" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I214" s="101"/>
+    </row>
+    <row r="215" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A215"/>
-    </row>
-    <row r="216" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I215" s="101"/>
+    </row>
+    <row r="216" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A216"/>
-    </row>
-    <row r="217" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I216" s="101"/>
+    </row>
+    <row r="217" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A217"/>
-    </row>
-    <row r="218" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I217" s="101"/>
+    </row>
+    <row r="218" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A218"/>
-    </row>
-    <row r="219" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I218" s="101"/>
+    </row>
+    <row r="219" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A219"/>
-    </row>
-    <row r="220" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I219" s="101"/>
+    </row>
+    <row r="220" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A220"/>
-    </row>
-    <row r="221" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I220" s="101"/>
+    </row>
+    <row r="221" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A221"/>
-    </row>
-    <row r="222" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I221" s="101"/>
+    </row>
+    <row r="222" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A222"/>
-    </row>
-    <row r="223" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I222" s="101"/>
+    </row>
+    <row r="223" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A223"/>
-    </row>
-    <row r="224" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I223" s="101"/>
+    </row>
+    <row r="224" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A224"/>
-    </row>
-    <row r="225" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I224" s="101"/>
+    </row>
+    <row r="225" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A225"/>
-    </row>
-    <row r="226" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I225" s="101"/>
+    </row>
+    <row r="226" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A226"/>
-    </row>
-    <row r="227" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I226" s="101"/>
+    </row>
+    <row r="227" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A227"/>
-    </row>
-    <row r="228" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I227" s="101"/>
+    </row>
+    <row r="228" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A228"/>
-    </row>
-    <row r="229" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I228" s="101"/>
+    </row>
+    <row r="229" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A229"/>
-    </row>
-    <row r="230" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I229" s="101"/>
+    </row>
+    <row r="230" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A230"/>
-    </row>
-    <row r="231" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I230" s="101"/>
+    </row>
+    <row r="231" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A231"/>
-    </row>
-    <row r="232" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I231" s="101"/>
+    </row>
+    <row r="232" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A232"/>
-    </row>
-    <row r="233" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I232" s="101"/>
+    </row>
+    <row r="233" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A233"/>
-    </row>
-    <row r="234" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I233" s="101"/>
+    </row>
+    <row r="234" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A234"/>
-    </row>
-    <row r="235" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I234" s="101"/>
+    </row>
+    <row r="235" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A235"/>
-    </row>
-    <row r="236" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I235" s="101"/>
+    </row>
+    <row r="236" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A236"/>
-    </row>
-    <row r="237" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I236" s="101"/>
+    </row>
+    <row r="237" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A237"/>
-    </row>
-    <row r="238" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I237" s="101"/>
+    </row>
+    <row r="238" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A238"/>
-    </row>
-    <row r="239" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I238" s="101"/>
+    </row>
+    <row r="239" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A239"/>
-    </row>
-    <row r="240" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I239" s="101"/>
+    </row>
+    <row r="240" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A240"/>
-    </row>
-    <row r="241" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I240" s="101"/>
+    </row>
+    <row r="241" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A241"/>
-    </row>
-    <row r="242" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I241" s="101"/>
+    </row>
+    <row r="242" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A242"/>
-    </row>
-    <row r="243" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I242" s="101"/>
+    </row>
+    <row r="243" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A243"/>
-    </row>
-    <row r="244" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I243" s="101"/>
+    </row>
+    <row r="244" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A244"/>
-    </row>
-    <row r="245" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I244" s="101"/>
+    </row>
+    <row r="245" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A245"/>
-    </row>
-    <row r="246" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I245" s="101"/>
+    </row>
+    <row r="246" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A246"/>
-    </row>
-    <row r="247" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I246" s="101"/>
+    </row>
+    <row r="247" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A247"/>
-    </row>
-    <row r="248" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I247" s="101"/>
+    </row>
+    <row r="248" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A248"/>
-    </row>
-    <row r="249" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I248" s="101"/>
+    </row>
+    <row r="249" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A249"/>
-    </row>
-    <row r="250" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I249" s="101"/>
+    </row>
+    <row r="250" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A250"/>
-    </row>
-    <row r="251" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I250" s="101"/>
+    </row>
+    <row r="251" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A251"/>
-    </row>
-    <row r="252" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I251" s="101"/>
+    </row>
+    <row r="252" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A252"/>
-    </row>
-    <row r="253" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I252" s="101"/>
+    </row>
+    <row r="253" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A253"/>
-    </row>
-    <row r="254" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I253" s="101"/>
+    </row>
+    <row r="254" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A254"/>
-    </row>
-    <row r="255" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I254" s="101"/>
+    </row>
+    <row r="255" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A255"/>
-    </row>
-    <row r="256" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I255" s="101"/>
+    </row>
+    <row r="256" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A256"/>
-    </row>
-    <row r="257" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I256" s="101"/>
+    </row>
+    <row r="257" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A257"/>
-    </row>
-    <row r="258" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I257" s="101"/>
+    </row>
+    <row r="258" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A258"/>
-    </row>
-    <row r="259" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I258" s="101"/>
+    </row>
+    <row r="259" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A259"/>
-    </row>
-    <row r="260" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I259" s="101"/>
+    </row>
+    <row r="260" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A260"/>
-    </row>
-    <row r="261" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I260" s="101"/>
+    </row>
+    <row r="261" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A261"/>
-    </row>
-    <row r="262" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I261" s="101"/>
+    </row>
+    <row r="262" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A262"/>
-    </row>
-    <row r="263" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I262" s="101"/>
+    </row>
+    <row r="263" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A263"/>
-    </row>
-    <row r="264" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I263" s="101"/>
+    </row>
+    <row r="264" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A264"/>
-    </row>
-    <row r="265" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I264" s="101"/>
+    </row>
+    <row r="265" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A265"/>
-    </row>
-    <row r="266" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I265" s="101"/>
+    </row>
+    <row r="266" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A266"/>
-    </row>
-    <row r="267" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I266" s="101"/>
+    </row>
+    <row r="267" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A267"/>
-    </row>
-    <row r="268" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I267" s="101"/>
+    </row>
+    <row r="268" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A268"/>
-    </row>
-    <row r="269" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I268" s="101"/>
+    </row>
+    <row r="269" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A269"/>
-    </row>
-    <row r="270" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I269" s="101"/>
+    </row>
+    <row r="270" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A270"/>
-    </row>
-    <row r="271" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I270" s="101"/>
+    </row>
+    <row r="271" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A271"/>
-    </row>
-    <row r="272" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I271" s="101"/>
+    </row>
+    <row r="272" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A272"/>
-    </row>
-    <row r="273" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I272" s="101"/>
+    </row>
+    <row r="273" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A273"/>
-    </row>
-    <row r="274" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I273" s="101"/>
+    </row>
+    <row r="274" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A274"/>
-    </row>
-    <row r="275" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I274" s="101"/>
+    </row>
+    <row r="275" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A275"/>
-    </row>
-    <row r="276" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I275" s="101"/>
+    </row>
+    <row r="276" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A276"/>
-    </row>
-    <row r="277" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I276" s="101"/>
+    </row>
+    <row r="277" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A277"/>
-    </row>
-    <row r="278" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I277" s="101"/>
+    </row>
+    <row r="278" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A278"/>
-    </row>
-    <row r="279" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I278" s="101"/>
+    </row>
+    <row r="279" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A279"/>
-    </row>
-    <row r="280" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I279" s="101"/>
+    </row>
+    <row r="280" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A280"/>
-    </row>
-    <row r="281" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I280" s="101"/>
+    </row>
+    <row r="281" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A281"/>
-    </row>
-    <row r="282" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I281" s="101"/>
+    </row>
+    <row r="282" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A282"/>
-    </row>
-    <row r="283" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I282" s="101"/>
+    </row>
+    <row r="283" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A283"/>
-    </row>
-    <row r="284" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I283" s="101"/>
+    </row>
+    <row r="284" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A284"/>
-    </row>
-    <row r="285" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I284" s="101"/>
+    </row>
+    <row r="285" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A285"/>
-    </row>
-    <row r="286" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I285" s="101"/>
+    </row>
+    <row r="286" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A286"/>
-    </row>
-    <row r="287" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I286" s="101"/>
+    </row>
+    <row r="287" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A287"/>
-    </row>
-    <row r="288" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I287" s="101"/>
+    </row>
+    <row r="288" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A288"/>
-    </row>
-    <row r="289" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I288" s="101"/>
+    </row>
+    <row r="289" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A289"/>
-    </row>
-    <row r="290" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I289" s="101"/>
+    </row>
+    <row r="290" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A290"/>
-    </row>
-    <row r="291" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I290" s="101"/>
+    </row>
+    <row r="291" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291"/>
-    </row>
-    <row r="292" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I291" s="101"/>
+    </row>
+    <row r="292" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A292"/>
-    </row>
-    <row r="293" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I292" s="101"/>
+    </row>
+    <row r="293" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A293"/>
-    </row>
-    <row r="294" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I293" s="101"/>
+    </row>
+    <row r="294" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A294"/>
-    </row>
-    <row r="295" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I294" s="101"/>
+    </row>
+    <row r="295" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A295"/>
-    </row>
-    <row r="296" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I295" s="101"/>
+    </row>
+    <row r="296" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A296"/>
-    </row>
-    <row r="297" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I296" s="101"/>
+    </row>
+    <row r="297" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A297"/>
-    </row>
-    <row r="298" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I297" s="101"/>
+    </row>
+    <row r="298" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A298"/>
-    </row>
-    <row r="299" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I298" s="101"/>
+    </row>
+    <row r="299" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A299"/>
-    </row>
-    <row r="300" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I299" s="101"/>
+    </row>
+    <row r="300" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A300"/>
-    </row>
-    <row r="301" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I300" s="101"/>
+    </row>
+    <row r="301" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A301"/>
-    </row>
-    <row r="302" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I301" s="101"/>
+    </row>
+    <row r="302" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A302"/>
-    </row>
-    <row r="303" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I302" s="101"/>
+    </row>
+    <row r="303" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A303"/>
-    </row>
-    <row r="304" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I303" s="101"/>
+    </row>
+    <row r="304" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A304"/>
-    </row>
-    <row r="305" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I304" s="101"/>
+    </row>
+    <row r="305" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A305"/>
-    </row>
-    <row r="306" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I305" s="101"/>
+    </row>
+    <row r="306" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A306"/>
-    </row>
-    <row r="307" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I306" s="101"/>
+    </row>
+    <row r="307" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A307"/>
-    </row>
-    <row r="308" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I307" s="101"/>
+    </row>
+    <row r="308" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A308"/>
-    </row>
-    <row r="309" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I308" s="101"/>
+    </row>
+    <row r="309" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A309"/>
-    </row>
-    <row r="310" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I309" s="101"/>
+    </row>
+    <row r="310" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A310"/>
-    </row>
-    <row r="311" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I310" s="101"/>
+    </row>
+    <row r="311" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A311"/>
-    </row>
-    <row r="312" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I311" s="101"/>
+    </row>
+    <row r="312" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A312"/>
-    </row>
-    <row r="313" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I312" s="101"/>
+    </row>
+    <row r="313" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A313"/>
-    </row>
-    <row r="314" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I313" s="101"/>
+    </row>
+    <row r="314" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A314"/>
-    </row>
-    <row r="315" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I314" s="101"/>
+    </row>
+    <row r="315" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A315"/>
-    </row>
-    <row r="316" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I315" s="101"/>
+    </row>
+    <row r="316" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A316"/>
-    </row>
-    <row r="317" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I316" s="101"/>
+    </row>
+    <row r="317" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A317"/>
-    </row>
-    <row r="318" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I317" s="101"/>
+    </row>
+    <row r="318" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A318"/>
-    </row>
-    <row r="319" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I318" s="101"/>
+    </row>
+    <row r="319" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A319"/>
-    </row>
-    <row r="320" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I319" s="101"/>
+    </row>
+    <row r="320" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A320"/>
-    </row>
-    <row r="321" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I320" s="101"/>
+    </row>
+    <row r="321" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A321"/>
-    </row>
-    <row r="322" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I321" s="101"/>
+    </row>
+    <row r="322" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A322"/>
-    </row>
-    <row r="323" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I322" s="101"/>
+    </row>
+    <row r="323" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A323"/>
-    </row>
-    <row r="324" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I323" s="101"/>
+    </row>
+    <row r="324" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A324"/>
-    </row>
-    <row r="325" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I324" s="101"/>
+    </row>
+    <row r="325" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A325"/>
-    </row>
-    <row r="326" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I325" s="101"/>
+    </row>
+    <row r="326" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A326"/>
-    </row>
-    <row r="327" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I326" s="101"/>
+    </row>
+    <row r="327" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A327"/>
-    </row>
-    <row r="328" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I327" s="101"/>
+    </row>
+    <row r="328" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A328"/>
-    </row>
-    <row r="329" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I328" s="101"/>
+    </row>
+    <row r="329" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A329"/>
-    </row>
-    <row r="330" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I329" s="101"/>
+    </row>
+    <row r="330" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A330"/>
-    </row>
-    <row r="331" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I330" s="101"/>
+    </row>
+    <row r="331" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A331"/>
-    </row>
-    <row r="332" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I331" s="101"/>
+    </row>
+    <row r="332" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A332"/>
-    </row>
-    <row r="333" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I332" s="101"/>
+    </row>
+    <row r="333" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A333"/>
-    </row>
-    <row r="334" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I333" s="101"/>
+    </row>
+    <row r="334" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A334"/>
-    </row>
-    <row r="335" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I334" s="101"/>
+    </row>
+    <row r="335" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A335"/>
-    </row>
-    <row r="336" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I335" s="101"/>
+    </row>
+    <row r="336" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A336"/>
-    </row>
-    <row r="337" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I336" s="101"/>
+    </row>
+    <row r="337" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A337"/>
-    </row>
-    <row r="338" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I337" s="101"/>
+    </row>
+    <row r="338" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A338"/>
-    </row>
-    <row r="339" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I338" s="101"/>
+    </row>
+    <row r="339" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A339"/>
-    </row>
-    <row r="340" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I339" s="101"/>
+    </row>
+    <row r="340" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A340"/>
-    </row>
-    <row r="341" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I340" s="101"/>
+    </row>
+    <row r="341" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A341"/>
-    </row>
-    <row r="342" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I341" s="101"/>
+    </row>
+    <row r="342" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A342"/>
-    </row>
-    <row r="343" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I342" s="101"/>
+    </row>
+    <row r="343" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A343"/>
-    </row>
-    <row r="344" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I343" s="101"/>
+    </row>
+    <row r="344" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A344"/>
-    </row>
-    <row r="345" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I344" s="101"/>
+    </row>
+    <row r="345" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A345"/>
-    </row>
-    <row r="346" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I345" s="101"/>
+    </row>
+    <row r="346" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A346"/>
-    </row>
-    <row r="347" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I346" s="101"/>
+    </row>
+    <row r="347" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A347"/>
-    </row>
-    <row r="348" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I347" s="101"/>
+    </row>
+    <row r="348" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A348"/>
-    </row>
-    <row r="349" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I348" s="101"/>
+    </row>
+    <row r="349" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A349"/>
-    </row>
-    <row r="350" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I349" s="101"/>
+    </row>
+    <row r="350" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A350"/>
-    </row>
-    <row r="351" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I350" s="101"/>
+    </row>
+    <row r="351" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A351"/>
-    </row>
-    <row r="352" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I351" s="101"/>
+    </row>
+    <row r="352" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A352"/>
-    </row>
-    <row r="353" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I352" s="101"/>
+    </row>
+    <row r="353" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A353"/>
-    </row>
-    <row r="354" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I353" s="101"/>
+    </row>
+    <row r="354" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A354"/>
-    </row>
-    <row r="355" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I354" s="101"/>
+    </row>
+    <row r="355" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A355"/>
-    </row>
-    <row r="356" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I355" s="101"/>
+    </row>
+    <row r="356" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A356"/>
-    </row>
-    <row r="357" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I356" s="101"/>
+    </row>
+    <row r="357" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A357"/>
-    </row>
-    <row r="358" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I357" s="101"/>
+    </row>
+    <row r="358" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A358"/>
-    </row>
-    <row r="359" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I358" s="101"/>
+    </row>
+    <row r="359" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A359"/>
-    </row>
-    <row r="360" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I359" s="101"/>
+    </row>
+    <row r="360" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360"/>
-    </row>
-    <row r="361" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I360" s="101"/>
+    </row>
+    <row r="361" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A361"/>
-    </row>
-    <row r="362" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I361" s="101"/>
+    </row>
+    <row r="362" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362"/>
-    </row>
-    <row r="363" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I362" s="101"/>
+    </row>
+    <row r="363" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A363"/>
-    </row>
-    <row r="364" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I363" s="101"/>
+    </row>
+    <row r="364" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A364"/>
-    </row>
-    <row r="365" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I364" s="101"/>
+    </row>
+    <row r="365" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A365"/>
-    </row>
-    <row r="366" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I365" s="101"/>
+    </row>
+    <row r="366" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A366"/>
-    </row>
-    <row r="367" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I366" s="101"/>
+    </row>
+    <row r="367" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A367"/>
-    </row>
-    <row r="368" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I367" s="101"/>
+    </row>
+    <row r="368" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368"/>
-    </row>
-    <row r="369" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I368" s="101"/>
+    </row>
+    <row r="369" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A369"/>
-    </row>
-    <row r="370" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I369" s="101"/>
+    </row>
+    <row r="370" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A370"/>
-    </row>
-    <row r="371" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I370" s="101"/>
+    </row>
+    <row r="371" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A371"/>
-    </row>
-    <row r="372" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I371" s="101"/>
+    </row>
+    <row r="372" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A372"/>
-    </row>
-    <row r="373" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I372" s="101"/>
+    </row>
+    <row r="373" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A373"/>
-    </row>
-    <row r="374" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I373" s="101"/>
+    </row>
+    <row r="374" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A374"/>
-    </row>
-    <row r="375" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I374" s="101"/>
+    </row>
+    <row r="375" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375"/>
-    </row>
-    <row r="376" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I375" s="101"/>
+    </row>
+    <row r="376" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A376"/>
-    </row>
-    <row r="377" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I376" s="101"/>
+    </row>
+    <row r="377" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A377"/>
-    </row>
-    <row r="378" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I377" s="101"/>
+    </row>
+    <row r="378" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A378"/>
-    </row>
-    <row r="379" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I378" s="101"/>
+    </row>
+    <row r="379" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A379"/>
-    </row>
-    <row r="380" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I379" s="101"/>
+    </row>
+    <row r="380" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A380"/>
-    </row>
-    <row r="381" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I380" s="101"/>
+    </row>
+    <row r="381" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381"/>
-    </row>
-    <row r="382" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I381" s="101"/>
+    </row>
+    <row r="382" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A382"/>
-    </row>
-    <row r="383" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I382" s="101"/>
+    </row>
+    <row r="383" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A383"/>
-    </row>
-    <row r="384" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I383" s="101"/>
+    </row>
+    <row r="384" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A384"/>
-    </row>
-    <row r="385" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I384" s="101"/>
+    </row>
+    <row r="385" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A385"/>
-    </row>
-    <row r="386" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I385" s="101"/>
+    </row>
+    <row r="386" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A386"/>
-    </row>
-    <row r="387" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I386" s="101"/>
+    </row>
+    <row r="387" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A387"/>
-    </row>
-    <row r="388" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I387" s="101"/>
+    </row>
+    <row r="388" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A388"/>
-    </row>
-    <row r="389" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I388" s="101"/>
+    </row>
+    <row r="389" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A389"/>
-    </row>
-    <row r="390" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I389" s="101"/>
+    </row>
+    <row r="390" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A390"/>
-    </row>
-    <row r="391" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I390" s="101"/>
+    </row>
+    <row r="391" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A391"/>
-    </row>
-    <row r="392" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I391" s="101"/>
+    </row>
+    <row r="392" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A392"/>
-    </row>
-    <row r="393" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I392" s="101"/>
+    </row>
+    <row r="393" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A393"/>
-    </row>
-    <row r="394" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I393" s="101"/>
+    </row>
+    <row r="394" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A394"/>
-    </row>
-    <row r="395" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I394" s="101"/>
+    </row>
+    <row r="395" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A395"/>
-    </row>
-    <row r="396" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I395" s="101"/>
+    </row>
+    <row r="396" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A396"/>
-    </row>
-    <row r="397" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I396" s="101"/>
+    </row>
+    <row r="397" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A397"/>
-    </row>
-    <row r="398" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I397" s="101"/>
+    </row>
+    <row r="398" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A398"/>
-    </row>
-    <row r="399" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I398" s="101"/>
+    </row>
+    <row r="399" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A399"/>
-    </row>
-    <row r="400" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I399" s="101"/>
+    </row>
+    <row r="400" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A400"/>
-    </row>
-    <row r="401" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I400" s="101"/>
+    </row>
+    <row r="401" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A401"/>
-    </row>
-    <row r="402" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I401" s="101"/>
+    </row>
+    <row r="402" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A402"/>
-    </row>
-    <row r="403" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I402" s="101"/>
+    </row>
+    <row r="403" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A403"/>
-    </row>
-    <row r="404" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I403" s="101"/>
+    </row>
+    <row r="404" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A404"/>
-    </row>
-    <row r="405" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I404" s="101"/>
+    </row>
+    <row r="405" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A405"/>
-    </row>
-    <row r="406" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I405" s="101"/>
+    </row>
+    <row r="406" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A406"/>
-    </row>
-    <row r="407" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I406" s="101"/>
+    </row>
+    <row r="407" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A407"/>
-    </row>
-    <row r="408" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I407" s="101"/>
+    </row>
+    <row r="408" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A408"/>
-    </row>
-    <row r="409" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I408" s="101"/>
+    </row>
+    <row r="409" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A409"/>
-    </row>
-    <row r="410" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I409" s="101"/>
+    </row>
+    <row r="410" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A410"/>
-    </row>
-    <row r="411" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I410" s="101"/>
+    </row>
+    <row r="411" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A411"/>
-    </row>
-    <row r="412" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I411" s="101"/>
+    </row>
+    <row r="412" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A412"/>
-    </row>
-    <row r="413" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I412" s="101"/>
+    </row>
+    <row r="413" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A413"/>
-    </row>
-    <row r="414" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I413" s="101"/>
+    </row>
+    <row r="414" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A414"/>
-    </row>
-    <row r="415" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I414" s="101"/>
+    </row>
+    <row r="415" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A415"/>
-    </row>
-    <row r="416" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I415" s="101"/>
+    </row>
+    <row r="416" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A416"/>
-    </row>
-    <row r="417" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I416" s="101"/>
+    </row>
+    <row r="417" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A417"/>
-    </row>
-    <row r="418" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I417" s="101"/>
+    </row>
+    <row r="418" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A418"/>
-    </row>
-    <row r="419" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I418" s="101"/>
+    </row>
+    <row r="419" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A419"/>
-    </row>
-    <row r="420" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I419" s="101"/>
+    </row>
+    <row r="420" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A420"/>
-    </row>
-    <row r="421" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I420" s="101"/>
+    </row>
+    <row r="421" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A421"/>
-    </row>
-    <row r="422" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I421" s="101"/>
+    </row>
+    <row r="422" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A422"/>
-    </row>
-    <row r="423" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I422" s="101"/>
+    </row>
+    <row r="423" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A423"/>
-    </row>
-    <row r="424" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I423" s="101"/>
+    </row>
+    <row r="424" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A424"/>
-    </row>
-    <row r="425" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I424" s="101"/>
+    </row>
+    <row r="425" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A425"/>
-    </row>
-    <row r="426" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I425" s="101"/>
+    </row>
+    <row r="426" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A426"/>
-    </row>
-    <row r="427" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I426" s="101"/>
+    </row>
+    <row r="427" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A427"/>
-    </row>
-    <row r="428" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I427" s="101"/>
+    </row>
+    <row r="428" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A428"/>
-    </row>
-    <row r="429" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I428" s="101"/>
+    </row>
+    <row r="429" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A429"/>
-    </row>
-    <row r="430" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I429" s="101"/>
+    </row>
+    <row r="430" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A430"/>
-    </row>
-    <row r="431" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I430" s="101"/>
+    </row>
+    <row r="431" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A431"/>
-    </row>
-    <row r="432" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I431" s="101"/>
+    </row>
+    <row r="432" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A432"/>
-    </row>
-    <row r="433" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I432" s="101"/>
+    </row>
+    <row r="433" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A433"/>
-    </row>
-    <row r="434" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I433" s="101"/>
+    </row>
+    <row r="434" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A434"/>
-    </row>
-    <row r="435" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I434" s="101"/>
+    </row>
+    <row r="435" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A435"/>
-    </row>
-    <row r="436" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I435" s="101"/>
+    </row>
+    <row r="436" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A436"/>
-    </row>
-    <row r="437" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I436" s="101"/>
+    </row>
+    <row r="437" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A437"/>
-    </row>
-    <row r="438" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I437" s="101"/>
+    </row>
+    <row r="438" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A438"/>
-    </row>
-    <row r="439" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I438" s="101"/>
+    </row>
+    <row r="439" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A439"/>
-    </row>
-    <row r="440" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I439" s="101"/>
+    </row>
+    <row r="440" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A440"/>
-    </row>
-    <row r="441" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I440" s="101"/>
+    </row>
+    <row r="441" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A441"/>
-    </row>
-    <row r="442" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I441" s="101"/>
+    </row>
+    <row r="442" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A442"/>
-    </row>
-    <row r="443" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I442" s="101"/>
+    </row>
+    <row r="443" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A443"/>
-    </row>
-    <row r="444" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I443" s="101"/>
+    </row>
+    <row r="444" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A444"/>
-    </row>
-    <row r="445" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I444" s="101"/>
+    </row>
+    <row r="445" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A445"/>
-    </row>
-    <row r="446" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I445" s="101"/>
+    </row>
+    <row r="446" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A446"/>
-    </row>
-    <row r="447" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I446" s="101"/>
+    </row>
+    <row r="447" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A447"/>
-    </row>
-    <row r="448" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I447" s="101"/>
+    </row>
+    <row r="448" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A448"/>
-    </row>
-    <row r="449" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I448" s="101"/>
+    </row>
+    <row r="449" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A449"/>
-    </row>
-    <row r="450" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I449" s="101"/>
+    </row>
+    <row r="450" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A450"/>
-    </row>
-    <row r="451" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I450" s="101"/>
+    </row>
+    <row r="451" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A451"/>
-    </row>
-    <row r="452" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I451" s="101"/>
+    </row>
+    <row r="452" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A452"/>
-    </row>
-    <row r="453" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I452" s="101"/>
+    </row>
+    <row r="453" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A453"/>
-    </row>
-    <row r="454" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I453" s="101"/>
+    </row>
+    <row r="454" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A454"/>
-    </row>
-    <row r="455" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I454" s="101"/>
+    </row>
+    <row r="455" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A455"/>
-    </row>
-    <row r="456" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I455" s="101"/>
+    </row>
+    <row r="456" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A456"/>
-    </row>
-    <row r="457" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I456" s="101"/>
+    </row>
+    <row r="457" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A457"/>
-    </row>
-    <row r="458" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I457" s="101"/>
+    </row>
+    <row r="458" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A458"/>
-    </row>
-    <row r="459" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I458" s="101"/>
+    </row>
+    <row r="459" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A459"/>
-    </row>
-    <row r="460" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I459" s="101"/>
+    </row>
+    <row r="460" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A460"/>
-    </row>
-    <row r="461" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I460" s="101"/>
+    </row>
+    <row r="461" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A461"/>
-    </row>
-    <row r="462" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I461" s="101"/>
+    </row>
+    <row r="462" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A462"/>
-    </row>
-    <row r="463" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I462" s="101"/>
+    </row>
+    <row r="463" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A463"/>
-    </row>
-    <row r="464" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I463" s="101"/>
+    </row>
+    <row r="464" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A464"/>
-    </row>
-    <row r="465" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I464" s="101"/>
+    </row>
+    <row r="465" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A465"/>
-    </row>
-    <row r="466" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I465" s="101"/>
+    </row>
+    <row r="466" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A466"/>
-    </row>
-    <row r="467" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I466" s="101"/>
+    </row>
+    <row r="467" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A467"/>
-    </row>
-    <row r="468" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I467" s="101"/>
+    </row>
+    <row r="468" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A468"/>
-    </row>
-    <row r="469" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I468" s="101"/>
+    </row>
+    <row r="469" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A469"/>
-    </row>
-    <row r="470" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I469" s="101"/>
+    </row>
+    <row r="470" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A470"/>
-    </row>
-    <row r="471" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I470" s="101"/>
+    </row>
+    <row r="471" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A471"/>
-    </row>
-    <row r="472" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I471" s="101"/>
+    </row>
+    <row r="472" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A472"/>
-    </row>
-    <row r="473" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I472" s="101"/>
+    </row>
+    <row r="473" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A473"/>
-    </row>
-    <row r="474" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I473" s="101"/>
+    </row>
+    <row r="474" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A474"/>
-    </row>
-    <row r="475" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I474" s="101"/>
+    </row>
+    <row r="475" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A475"/>
-    </row>
-    <row r="476" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I475" s="101"/>
+    </row>
+    <row r="476" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A476"/>
-    </row>
-    <row r="477" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I476" s="101"/>
+    </row>
+    <row r="477" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A477"/>
-    </row>
-    <row r="478" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I477" s="101"/>
+    </row>
+    <row r="478" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A478"/>
-    </row>
-    <row r="479" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I478" s="101"/>
+    </row>
+    <row r="479" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A479"/>
-    </row>
-    <row r="480" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I479" s="101"/>
+    </row>
+    <row r="480" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A480"/>
-    </row>
-    <row r="481" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I480" s="101"/>
+    </row>
+    <row r="481" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A481"/>
-    </row>
-    <row r="482" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I481" s="101"/>
+    </row>
+    <row r="482" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A482"/>
-    </row>
-    <row r="483" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I482" s="101"/>
+    </row>
+    <row r="483" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A483"/>
-    </row>
-    <row r="484" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I483" s="101"/>
+    </row>
+    <row r="484" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A484"/>
-    </row>
-    <row r="485" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I484" s="101"/>
+    </row>
+    <row r="485" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A485"/>
-    </row>
-    <row r="486" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I485" s="101"/>
+    </row>
+    <row r="486" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A486"/>
-    </row>
-    <row r="487" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I486" s="101"/>
+    </row>
+    <row r="487" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A487"/>
-    </row>
-    <row r="488" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I487" s="101"/>
+    </row>
+    <row r="488" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A488"/>
-    </row>
-    <row r="489" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I488" s="101"/>
+    </row>
+    <row r="489" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A489"/>
-    </row>
-    <row r="490" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I489" s="101"/>
+    </row>
+    <row r="490" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A490"/>
-    </row>
-    <row r="491" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I490" s="101"/>
+    </row>
+    <row r="491" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A491"/>
-    </row>
-    <row r="492" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I491" s="101"/>
+    </row>
+    <row r="492" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A492"/>
-    </row>
-    <row r="493" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I492" s="101"/>
+    </row>
+    <row r="493" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A493"/>
-    </row>
-    <row r="494" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I493" s="101"/>
+    </row>
+    <row r="494" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A494"/>
-    </row>
-    <row r="495" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I494" s="101"/>
+    </row>
+    <row r="495" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A495"/>
-    </row>
-    <row r="496" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I495" s="101"/>
+    </row>
+    <row r="496" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A496"/>
-    </row>
-    <row r="497" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I496" s="101"/>
+    </row>
+    <row r="497" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A497"/>
-    </row>
-    <row r="498" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I497" s="101"/>
+    </row>
+    <row r="498" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A498"/>
-    </row>
-    <row r="499" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I498" s="101"/>
+    </row>
+    <row r="499" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A499"/>
-    </row>
-    <row r="500" spans="1:1" s="100" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I499" s="101"/>
+    </row>
+    <row r="500" spans="1:9" s="100" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A500"/>
+      <c r="I500" s="101"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>